<commit_message>
plotted all year fluxes and rates
</commit_message>
<xml_diff>
--- a/data/flux/2018-fluxes.xlsx
+++ b/data/flux/2018-fluxes.xlsx
@@ -21,324 +21,333 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="112">
   <si>
     <t xml:space="preserve">sample id</t>
   </si>
   <si>
+    <t xml:space="preserve">Station</t>
+  </si>
+  <si>
     <t xml:space="preserve">Year</t>
   </si>
   <si>
-    <t xml:space="preserve">Station</t>
+    <t xml:space="preserve">Depth (m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure [dbar]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trap type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flux (mg/m2/day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:N organic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Org C flux (umol C/m2/day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protein flux (ug/m2/day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbon protein flux (umol C/m2/day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N production rate (nM N/day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-30_151m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-30_151m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-31_121m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-31_121m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-32_147m_top_remainder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-32_147m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-32_147m_+P_remainder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-32_147m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-32_147m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-32_147m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-32_147m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-32_147m_nw4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_368m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_368m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_368m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_368m_nw1 (does this exist?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_368m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_368m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_586m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_586m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_586m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_586m_nw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-34_87m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-34_87m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-34_87m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-34_221m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-34_221m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-34_221m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-36_85m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-36_85m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-36_85m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-36_85m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-36_85m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-36_85m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-36_147m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-36_147m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-37_50m_+P1/top1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-37_50m_+P/top2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-37_50m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-37_50m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-37_120m_+P/top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-37_120m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-37_120m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-37_120m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-37_120m_nw4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-38_122m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-38_122m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-38_122m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-39_120m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-39_190m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-39_190m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-39_190m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_123m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_123m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_123m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_123m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_201m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_201m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_201m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_201m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_201m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_201m_nw4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_201m_nw5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_221m_+P1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_221m_+P2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_221m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_221m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_221m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_221m_nw4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_586m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_586m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_586m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_586m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_586m_nw4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-43_145m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-43_145m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-43_145m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-43_288m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-44_93m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-44_93m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-44_93m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_143m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_143m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_143m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_143m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_143m_nw4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_143m_nw5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_843m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_843m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_843m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_843m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_843m_nw4</t>
   </si>
   <si>
     <t xml:space="preserve">Depth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pressure [dbar]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flux (mg/m2/day)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C flux organic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trap type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CN total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CN organic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-30_151m_+P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-30_151m_ctl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-31_121m_+P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-31_121m_ctl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-32_147m_top_remainder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">net</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-32_147m_top</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-32_147m_+P_remainder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-32_147m_ctl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-32_147m_nw1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-32_147m_nw2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-32_147m_nw3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-32_147m_nw4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-33_368m_top</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-33_368m_+P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-33_368m_ctl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-33_368m_nw1 (does this exist?)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-33_368m_nw2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-33_368m_nw3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-33_586m_top</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-33_586m_+P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-33_586m_ctl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-33_586m_nw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-34_87m_top</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-34_87m_+P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-34_87m_ctl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-34_221m_top</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-34_221m_+P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-34_221m_ctl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-36_85m_top</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-36_85m_+P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-36_85m_ctl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-36_85m_nw1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-36_85m_nw2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-36_85m_nw3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-36_147m_nw1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-36_147m_nw2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-37_50m_+P1/top1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-37_50m_+P/top2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-37_50m_nw1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-37_50m_nw2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-37_120m_+P/top</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-37_120m_nw1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-37_120m_nw2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-37_120m_nw3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-37_120m_nw4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-38_122m_top</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-38_122m_+P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-38_122m_ctl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-39_120m_top</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-39_190m_top</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-39_190m_+P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-39_190m_ctl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-40_123m_+P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-40_123m_nw1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-40_123m_nw2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-40_123m_nw3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-40_201m_+P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-40_201m_ctl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-40_201m_nw1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-40_201m_nw2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-40_201m_nw3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-40_201m_nw4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-40_201m_nw5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-42_221m_+P1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-42_221m_+P2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-42_221m_nw1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-42_221m_nw2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-42_221m_nw3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-42_221m_nw4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-42_586m_+P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-42_586m_nw1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-42_586m_nw2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-42_586m_nw3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-42_586m_nw4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-43_145m_top</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-43_145m_+P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-43_145m_ctl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-43_288m_+P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-44_93m_top</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-44_93m_+P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-44_93m_ctl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-45_143m_+P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-45_143m_nw1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-45_143m_nw2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-45_143m_nw3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-45_143m_nw4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-45_143m_nw5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-45_843m_+P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-45_843m_nw1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-45_843m_nw2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-45_843m_nw3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-45_843m_nw4</t>
   </si>
   <si>
     <t xml:space="preserve">Fz C flux organic</t>
@@ -438,8 +447,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -519,7 +532,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart61.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -720,11 +733,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="27133868"/>
-        <c:axId val="42532551"/>
+        <c:axId val="42389324"/>
+        <c:axId val="25263661"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="27133868"/>
+        <c:axId val="42389324"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -780,12 +793,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42532551"/>
+        <c:crossAx val="25263661"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42532551"/>
+        <c:axId val="25263661"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -850,7 +863,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27133868"/>
+        <c:crossAx val="42389324"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -898,7 +911,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart62.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1069,11 +1082,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="63987704"/>
-        <c:axId val="99356231"/>
+        <c:axId val="4628659"/>
+        <c:axId val="62961195"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63987704"/>
+        <c:axId val="4628659"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1129,12 +1142,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99356231"/>
+        <c:crossAx val="62961195"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99356231"/>
+        <c:axId val="62961195"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1199,7 +1212,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63987704"/>
+        <c:crossAx val="4628659"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1247,7 +1260,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart63.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1448,11 +1461,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="41804782"/>
-        <c:axId val="21395595"/>
+        <c:axId val="34787098"/>
+        <c:axId val="55617147"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="41804782"/>
+        <c:axId val="34787098"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1508,12 +1521,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21395595"/>
+        <c:crossAx val="55617147"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="21395595"/>
+        <c:axId val="55617147"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1578,7 +1591,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41804782"/>
+        <c:crossAx val="34787098"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1626,7 +1639,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart64.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1797,11 +1810,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="79690787"/>
-        <c:axId val="51389328"/>
+        <c:axId val="16626035"/>
+        <c:axId val="66205091"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79690787"/>
+        <c:axId val="16626035"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1857,12 +1870,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51389328"/>
+        <c:crossAx val="66205091"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51389328"/>
+        <c:axId val="66205091"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1927,7 +1940,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79690787"/>
+        <c:crossAx val="16626035"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1986,9 +1999,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>719280</xdr:colOff>
+      <xdr:colOff>718920</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>84960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1996,8 +2009,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5065560" y="86040"/>
-        <a:ext cx="5437800" cy="4550760"/>
+        <a:off x="5073120" y="86040"/>
+        <a:ext cx="5445000" cy="4550400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2016,9 +2029,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>225720</xdr:colOff>
+      <xdr:colOff>225360</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2026,8 +2039,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5058720" y="4924800"/>
-        <a:ext cx="4951080" cy="4722840"/>
+        <a:off x="5066280" y="4924800"/>
+        <a:ext cx="4958280" cy="4722480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2046,9 +2059,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>605520</xdr:colOff>
+      <xdr:colOff>605160</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>161640</xdr:rowOff>
+      <xdr:rowOff>161280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2056,8 +2069,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10658880" y="0"/>
-        <a:ext cx="5437800" cy="4550760"/>
+        <a:off x="10675440" y="0"/>
+        <a:ext cx="5445000" cy="4550400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2076,9 +2089,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>99000</xdr:colOff>
+      <xdr:colOff>98640</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>104760</xdr:rowOff>
+      <xdr:rowOff>104400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2086,8 +2099,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10639080" y="4972680"/>
-        <a:ext cx="4951080" cy="4722840"/>
+        <a:off x="10655640" y="4972680"/>
+        <a:ext cx="4958280" cy="4722480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2105,22 +2118,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J93"/>
+  <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E96" activeCellId="0" sqref="E96"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="15.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2154,2267 +2169,2147 @@
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>151</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="2" t="n">
         <v>151</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>59.93179319</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="H2" s="0" t="n">
+        <v>12.3127516778524</v>
+      </c>
+      <c r="I2" s="0" t="n">
         <v>114.4817664</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>22.2485089463221</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>12.3127516778524</v>
+      <c r="L2" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>11</v>
+      <c r="C3" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>151</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>151</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>130.114754098361</v>
-      </c>
-      <c r="J3" s="0" t="n">
+      <c r="F3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="0" t="n">
         <v>58.1495726495727</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>121</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="2" t="n">
         <v>121</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="0" t="n">
         <v>140.2346446</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="H4" s="0" t="n">
+        <v>25.7815533980582</v>
+      </c>
+      <c r="I4" s="0" t="n">
         <v>142.1919526</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>30.9538461538461</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>25.7815533980582</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>121</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="2" t="n">
         <v>121</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>16.058981233244</v>
-      </c>
-      <c r="J5" s="0" t="n">
+      <c r="F5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="0" t="n">
         <v>76.4009433962264</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>147</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="2" t="n">
         <v>147</v>
       </c>
-      <c r="H6" s="0" t="s">
-        <v>17</v>
+      <c r="F6" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>11</v>
+        <v>20</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>147</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="2" t="n">
         <v>147</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <v>135.5691057</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="I7" s="0" t="n">
         <v>6.088336976</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>11</v>
+        <v>21</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>147</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="2" t="n">
         <v>147</v>
       </c>
-      <c r="H8" s="0" t="s">
-        <v>17</v>
+      <c r="F8" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>11</v>
+        <v>22</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>147</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="2" t="n">
         <v>147</v>
       </c>
-      <c r="H9" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>50.0230769230769</v>
-      </c>
-      <c r="J9" s="0" t="n">
+      <c r="F9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="0" t="n">
         <v>20.0629370629371</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>147</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="2" t="n">
         <v>147</v>
       </c>
-      <c r="H10" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>9.83925979680697</v>
-      </c>
-      <c r="J10" s="0" t="n">
+      <c r="F10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="0" t="n">
         <v>9.29615547106041</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>147</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="2" t="n">
         <v>147</v>
       </c>
-      <c r="H11" s="0" t="s">
-        <v>17</v>
+      <c r="F11" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>147</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="2" t="n">
         <v>147</v>
       </c>
-      <c r="H12" s="0" t="s">
-        <v>17</v>
+      <c r="F12" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>147</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="2" t="n">
         <v>147</v>
       </c>
-      <c r="H13" s="0" t="s">
-        <v>17</v>
+      <c r="F13" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>368</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="2" t="n">
         <v>368</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="0" t="n">
         <v>5.577733349</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="H14" s="0" t="n">
+        <v>6.00653518496908</v>
+      </c>
+      <c r="I14" s="0" t="n">
         <v>36.77803059</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>7.51376623376623</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <v>6.00653518496908</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>11</v>
+        <v>28</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>368</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="2" t="n">
         <v>368</v>
       </c>
-      <c r="H15" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="0" t="n">
-        <v>10.098878695209</v>
-      </c>
-      <c r="J15" s="0" t="n">
+      <c r="F15" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="0" t="n">
         <v>7.78433862433862</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>375</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>11</v>
+        <v>29</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>368</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="E16" s="2" t="n">
         <v>368</v>
       </c>
-      <c r="H16" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J16" s="0" t="n">
+      <c r="F16" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="0" t="n">
         <v>31.2538461538462</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>11</v>
+        <v>30</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>368</v>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" s="2" t="n">
         <v>368</v>
       </c>
-      <c r="H17" s="0" t="s">
-        <v>17</v>
+      <c r="F17" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>368</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="2" t="n">
         <v>368</v>
       </c>
-      <c r="H18" s="0" t="s">
-        <v>17</v>
+      <c r="F18" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>368</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" s="2" t="n">
         <v>368</v>
       </c>
-      <c r="H19" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="0" t="n">
-        <v>8.47885304659498</v>
-      </c>
-      <c r="J19" s="0" t="n">
+      <c r="F19" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="0" t="n">
         <v>7.1683748169839</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>11</v>
+        <v>33</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>586</v>
       </c>
-      <c r="E20" s="1" t="n">
+      <c r="E20" s="2" t="n">
         <v>586</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="0" t="n">
         <v>8.164440297</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="H20" s="0" t="n">
+        <v>8.00515093435553</v>
+      </c>
+      <c r="I20" s="0" t="n">
         <v>49.69913676</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="0" t="n">
-        <v>9.82647754137116</v>
-      </c>
-      <c r="J20" s="0" t="n">
-        <v>8.00515093435553</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>11</v>
+        <v>34</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>586</v>
       </c>
-      <c r="E21" s="1" t="n">
+      <c r="E21" s="2" t="n">
         <v>586</v>
       </c>
-      <c r="H21" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="0" t="n">
-        <v>8.20273461777501</v>
-      </c>
-      <c r="J21" s="0" t="n">
+      <c r="F21" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="0" t="n">
         <v>7.24497117232543</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>11</v>
+        <v>35</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>586</v>
       </c>
-      <c r="E22" s="1" t="n">
+      <c r="E22" s="2" t="n">
         <v>586</v>
       </c>
-      <c r="H22" s="0" t="s">
-        <v>17</v>
+      <c r="F22" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>11</v>
+        <v>36</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>586</v>
       </c>
-      <c r="E23" s="1" t="n">
+      <c r="E23" s="2" t="n">
         <v>586</v>
       </c>
-      <c r="H23" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="0" t="n">
-        <v>11.8938313050776</v>
-      </c>
-      <c r="J23" s="0" t="n">
+      <c r="F23" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="0" t="n">
         <v>10.5844394527262</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>11</v>
+        <v>37</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>87</v>
       </c>
-      <c r="E24" s="1" t="n">
+      <c r="E24" s="2" t="n">
         <v>87</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="0" t="n">
         <v>24.18012422</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="H24" s="0" t="n">
+        <v>4.72782874617737</v>
+      </c>
+      <c r="I24" s="0" t="n">
         <v>54.81517583</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I24" s="0" t="n">
-        <v>5.80789170506912</v>
-      </c>
-      <c r="J24" s="0" t="n">
-        <v>4.72782874617737</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>11</v>
+        <v>38</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>87</v>
       </c>
-      <c r="E25" s="1" t="n">
+      <c r="E25" s="2" t="n">
         <v>87</v>
       </c>
-      <c r="H25" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I25" s="0" t="n">
-        <v>9.78732545649839</v>
-      </c>
-      <c r="J25" s="0" t="n">
+      <c r="F25" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="0" t="n">
         <v>4.95272525027809</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <v>38.5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>11</v>
+        <v>39</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>87</v>
       </c>
-      <c r="E26" s="1" t="n">
+      <c r="E26" s="2" t="n">
         <v>87</v>
       </c>
-      <c r="H26" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I26" s="0" t="n">
-        <v>28.0041666666667</v>
-      </c>
-      <c r="J26" s="0" t="n">
+      <c r="F26" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="0" t="n">
         <v>10.8071895424837</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>11</v>
+        <v>40</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>221</v>
       </c>
-      <c r="E27" s="1" t="n">
+      <c r="E27" s="2" t="n">
         <v>221</v>
       </c>
-      <c r="H27" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I27" s="0" t="n">
-        <v>14.8540669856459</v>
-      </c>
-      <c r="J27" s="0" t="n">
+      <c r="F27" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="0" t="n">
         <v>11.6933911159263</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>11</v>
+        <v>41</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>221</v>
       </c>
-      <c r="E28" s="1" t="n">
+      <c r="E28" s="2" t="n">
         <v>221</v>
       </c>
-      <c r="H28" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I28" s="0" t="n">
-        <v>22.0023201856149</v>
-      </c>
-      <c r="J28" s="0" t="n">
+      <c r="F28" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="0" t="n">
         <v>2.63057324840764</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>11</v>
+        <v>42</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>221</v>
       </c>
-      <c r="E29" s="1" t="n">
+      <c r="E29" s="2" t="n">
         <v>221</v>
       </c>
-      <c r="H29" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="J29" s="0" t="n">
+      <c r="F29" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="0" t="n">
         <v>5.58258642765685</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>11</v>
+        <v>43</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="E30" s="1" t="n">
+      <c r="E30" s="2" t="n">
         <v>85</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="0" t="n">
         <v>26.58868425</v>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="H30" s="0" t="n">
+        <v>6.12341352528888</v>
+      </c>
+      <c r="I30" s="0" t="n">
         <v>115.1818194</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="0" t="n">
-        <v>6.86597467776891</v>
-      </c>
-      <c r="J30" s="0" t="n">
-        <v>6.12341352528888</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="E31" s="1" t="n">
+      <c r="E31" s="2" t="n">
         <v>85</v>
       </c>
-      <c r="H31" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="0" t="n">
-        <v>5.64466430399685</v>
-      </c>
-      <c r="J31" s="0" t="n">
+      <c r="F31" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31" s="0" t="n">
         <v>5.66409124356144</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>530</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>11</v>
+        <v>45</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="E32" s="1" t="n">
+      <c r="E32" s="2" t="n">
         <v>85</v>
       </c>
-      <c r="H32" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J32" s="0" t="n">
+      <c r="F32" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" s="0" t="n">
         <v>13.2683760683761</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>11</v>
+        <v>46</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="E33" s="1" t="n">
+      <c r="E33" s="2" t="n">
         <v>85</v>
       </c>
-      <c r="H33" s="0" t="s">
-        <v>17</v>
+      <c r="F33" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>11</v>
+        <v>47</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="E34" s="1" t="n">
+      <c r="E34" s="2" t="n">
         <v>85</v>
       </c>
-      <c r="H34" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I34" s="0" t="n">
-        <v>7.9231573444851</v>
-      </c>
-      <c r="J34" s="0" t="n">
+      <c r="F34" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34" s="0" t="n">
         <v>8.43557336621455</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>11</v>
+        <v>48</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="E35" s="1" t="n">
+      <c r="E35" s="2" t="n">
         <v>85</v>
       </c>
-      <c r="H35" s="0" t="s">
-        <v>17</v>
+      <c r="F35" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>11</v>
+        <v>49</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>147</v>
       </c>
-      <c r="E36" s="1" t="n">
+      <c r="E36" s="2" t="n">
         <v>147</v>
       </c>
-      <c r="H36" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I36" s="0" t="n">
-        <v>7.65361077111383</v>
-      </c>
-      <c r="J36" s="0" t="n">
+      <c r="F36" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H36" s="0" t="n">
         <v>6.97915798249271</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B37" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>11</v>
+        <v>50</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>147</v>
       </c>
-      <c r="E37" s="1" t="n">
+      <c r="E37" s="2" t="n">
         <v>147</v>
       </c>
-      <c r="H37" s="0" t="s">
-        <v>17</v>
+      <c r="F37" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B38" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="E38" s="1" t="n">
+      <c r="E38" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="G38" s="0" t="n">
+      <c r="F38" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="0" t="n">
+        <v>6.7035458711908</v>
+      </c>
+      <c r="I38" s="0" t="n">
         <v>244.4055742</v>
-      </c>
-      <c r="H38" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I38" s="0" t="n">
-        <v>7.9217078481492</v>
-      </c>
-      <c r="J38" s="0" t="n">
-        <v>6.7035458711908</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="E39" s="1" t="n">
+      <c r="E39" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="H39" s="0" t="s">
-        <v>17</v>
+      <c r="F39" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="E40" s="1" t="n">
+      <c r="E40" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="H40" s="0" t="s">
-        <v>17</v>
+      <c r="F40" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="E41" s="1" t="n">
+      <c r="E41" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="H41" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I41" s="0" t="n">
-        <v>8.61121495327103</v>
-      </c>
-      <c r="J41" s="0" t="n">
+      <c r="F41" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H41" s="0" t="n">
         <v>7.96274373259053</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>50</v>
+        <v>56</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="E42" s="1" t="n">
+      <c r="E42" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="H42" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I42" s="0" t="n">
-        <v>8.04856475300401</v>
-      </c>
-      <c r="J42" s="0" t="n">
+      <c r="F42" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H42" s="0" t="n">
         <v>6.35134728285413</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B43" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>50</v>
+        <v>57</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="E43" s="1" t="n">
+      <c r="E43" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="H43" s="0" t="s">
-        <v>17</v>
+      <c r="F43" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B44" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>50</v>
+        <v>58</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="E44" s="1" t="n">
+      <c r="E44" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="H44" s="0" t="s">
-        <v>17</v>
+      <c r="F44" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B45" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>50</v>
+        <v>59</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="E45" s="1" t="n">
+      <c r="E45" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="H45" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I45" s="0" t="n">
-        <v>7.81244700695269</v>
-      </c>
-      <c r="J45" s="0" t="n">
+      <c r="F45" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H45" s="0" t="n">
         <v>7.10068803490519</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>50</v>
+        <v>60</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="E46" s="1" t="n">
+      <c r="E46" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="H46" s="0" t="s">
-        <v>17</v>
+      <c r="F46" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>50</v>
+        <v>61</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>122</v>
       </c>
-      <c r="E47" s="1" t="n">
+      <c r="E47" s="2" t="n">
         <v>122</v>
       </c>
-      <c r="F47" s="0" t="n">
+      <c r="F47" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" s="0" t="n">
         <v>32.66219522</v>
       </c>
-      <c r="G47" s="0" t="n">
+      <c r="H47" s="0" t="n">
+        <v>6.43644805571677</v>
+      </c>
+      <c r="I47" s="0" t="n">
         <v>48.90482028</v>
-      </c>
-      <c r="H47" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I47" s="0" t="n">
-        <v>7.64022346368715</v>
-      </c>
-      <c r="J47" s="0" t="n">
-        <v>6.43644805571677</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B48" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>50</v>
+        <v>62</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>122</v>
       </c>
-      <c r="E48" s="1" t="n">
+      <c r="E48" s="2" t="n">
         <v>122</v>
       </c>
-      <c r="H48" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I48" s="0" t="n">
-        <v>11.798459563543</v>
-      </c>
-      <c r="J48" s="0" t="n">
+      <c r="F48" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48" s="0" t="n">
         <v>2.96830864622804</v>
+      </c>
+      <c r="L48" s="0" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B49" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>50</v>
+        <v>63</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>122</v>
       </c>
-      <c r="E49" s="1" t="n">
+      <c r="E49" s="2" t="n">
         <v>122</v>
       </c>
-      <c r="H49" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I49" s="0" t="n">
-        <v>10.4847161572052</v>
-      </c>
-      <c r="J49" s="0" t="n">
+      <c r="F49" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H49" s="0" t="n">
         <v>9.47640449438202</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B50" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>50</v>
+        <v>64</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="E50" s="1" t="n">
+      <c r="E50" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="F50" s="0" t="n">
+      <c r="F50" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" s="0" t="n">
         <v>144.5962733</v>
       </c>
-      <c r="G50" s="0" t="n">
+      <c r="I50" s="0" t="n">
         <v>47.19008443</v>
-      </c>
-      <c r="H50" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I50" s="0" t="n">
-        <v>10.8403669724771</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B51" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>50</v>
+        <v>65</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>190</v>
       </c>
-      <c r="E51" s="1" t="n">
+      <c r="E51" s="2" t="n">
         <v>190</v>
       </c>
-      <c r="F51" s="0" t="n">
+      <c r="F51" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G51" s="0" t="n">
         <v>31.86596927</v>
       </c>
-      <c r="G51" s="0" t="n">
+      <c r="H51" s="0" t="n">
+        <v>5.58032128514056</v>
+      </c>
+      <c r="I51" s="0" t="n">
         <v>24.84261045</v>
-      </c>
-      <c r="H51" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I51" s="0" t="n">
-        <v>17.6749226006192</v>
-      </c>
-      <c r="J51" s="0" t="n">
-        <v>5.58032128514056</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>50</v>
+        <v>66</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>190</v>
       </c>
-      <c r="E52" s="1" t="n">
+      <c r="E52" s="2" t="n">
         <v>190</v>
       </c>
-      <c r="H52" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I52" s="0" t="n">
-        <v>11.3988355167394</v>
-      </c>
-      <c r="J52" s="0" t="n">
+      <c r="F52" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H52" s="0" t="n">
         <v>4.91321499013807</v>
+      </c>
+      <c r="L52" s="0" t="n">
+        <v>64</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B53" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>50</v>
+        <v>67</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>190</v>
       </c>
-      <c r="E53" s="1" t="n">
+      <c r="E53" s="2" t="n">
         <v>190</v>
       </c>
-      <c r="H53" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I53" s="0" t="n">
-        <v>21.3305439330544</v>
-      </c>
-      <c r="J53" s="0" t="n">
+      <c r="F53" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H53" s="0" t="n">
         <v>2.77491749174917</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B54" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>50</v>
+        <v>68</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>123</v>
       </c>
-      <c r="E54" s="1" t="n">
+      <c r="E54" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="F54" s="0" t="n">
+      <c r="F54" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G54" s="0" t="n">
         <v>127.6422764</v>
-      </c>
-      <c r="H54" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B55" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>50</v>
+        <v>69</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>123</v>
       </c>
-      <c r="E55" s="1" t="n">
+      <c r="E55" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="H55" s="0" t="s">
-        <v>17</v>
+      <c r="F55" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B56" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>50</v>
+        <v>70</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>123</v>
       </c>
-      <c r="E56" s="1" t="n">
+      <c r="E56" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="H56" s="0" t="s">
-        <v>17</v>
+      <c r="F56" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="B57" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>50</v>
+        <v>71</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>123</v>
       </c>
-      <c r="E57" s="1" t="n">
+      <c r="E57" s="2" t="n">
         <v>123</v>
       </c>
-      <c r="H57" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I57" s="0" t="n">
-        <v>8.64847089773101</v>
-      </c>
-      <c r="J57" s="0" t="n">
+      <c r="F57" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H57" s="0" t="n">
         <v>8.21664180341455</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B58" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>50</v>
+        <v>72</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>201</v>
       </c>
-      <c r="E58" s="1" t="n">
+      <c r="E58" s="2" t="n">
         <v>201</v>
       </c>
-      <c r="F58" s="0" t="n">
+      <c r="F58" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G58" s="0" t="n">
         <v>18.53988134</v>
       </c>
-      <c r="G58" s="0" t="n">
+      <c r="H58" s="0" t="n">
+        <v>6.92031090523671</v>
+      </c>
+      <c r="I58" s="0" t="n">
         <v>206.4532045</v>
-      </c>
-      <c r="H58" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I58" s="0" t="n">
-        <v>7.75922800322888</v>
-      </c>
-      <c r="J58" s="0" t="n">
-        <v>6.92031090523671</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B59" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C59" s="0" t="s">
-        <v>50</v>
+        <v>73</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>201</v>
       </c>
-      <c r="E59" s="1" t="n">
+      <c r="E59" s="2" t="n">
         <v>201</v>
       </c>
-      <c r="H59" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I59" s="0" t="n">
-        <v>33.8181818181818</v>
-      </c>
-      <c r="J59" s="0" t="n">
+      <c r="F59" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H59" s="0" t="n">
         <v>13.01269035533</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="B60" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>50</v>
+        <v>74</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>201</v>
       </c>
-      <c r="E60" s="1" t="n">
+      <c r="E60" s="2" t="n">
         <v>201</v>
       </c>
-      <c r="H60" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I60" s="0" t="n">
-        <v>8.79878923052413</v>
-      </c>
-      <c r="J60" s="0" t="n">
+      <c r="F60" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H60" s="0" t="n">
         <v>8.47593418422267</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B61" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>50</v>
+        <v>75</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>201</v>
       </c>
-      <c r="E61" s="1" t="n">
+      <c r="E61" s="2" t="n">
         <v>201</v>
       </c>
-      <c r="H61" s="0" t="s">
-        <v>17</v>
+      <c r="F61" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="B62" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>50</v>
+        <v>76</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D62" s="0" t="n">
         <v>201</v>
       </c>
-      <c r="E62" s="1" t="n">
+      <c r="E62" s="2" t="n">
         <v>201</v>
       </c>
-      <c r="H62" s="0" t="s">
-        <v>17</v>
+      <c r="F62" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B63" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>50</v>
+        <v>77</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D63" s="0" t="n">
         <v>201</v>
       </c>
-      <c r="E63" s="1" t="n">
+      <c r="E63" s="2" t="n">
         <v>201</v>
       </c>
-      <c r="H63" s="0" t="s">
-        <v>17</v>
+      <c r="F63" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="B64" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C64" s="0" t="s">
-        <v>50</v>
+        <v>78</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>201</v>
       </c>
-      <c r="E64" s="1" t="n">
+      <c r="E64" s="2" t="n">
         <v>201</v>
       </c>
-      <c r="H64" s="0" t="s">
-        <v>17</v>
+      <c r="F64" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="B65" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>50</v>
+        <v>79</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>221</v>
       </c>
-      <c r="E65" s="1" t="n">
+      <c r="E65" s="2" t="n">
         <v>221</v>
       </c>
-      <c r="H65" s="0" t="s">
-        <v>17</v>
+      <c r="F65" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="B66" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>50</v>
+        <v>80</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>221</v>
       </c>
-      <c r="E66" s="1" t="n">
+      <c r="E66" s="2" t="n">
         <v>221</v>
       </c>
-      <c r="F66" s="0" t="n">
+      <c r="F66" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G66" s="0" t="n">
         <v>7.360697997</v>
       </c>
-      <c r="G66" s="0" t="n">
+      <c r="H66" s="0" t="n">
+        <v>6.82834475297512</v>
+      </c>
+      <c r="I66" s="0" t="n">
         <v>94.40429427</v>
-      </c>
-      <c r="H66" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I66" s="0" t="n">
-        <v>8.34077131432994</v>
-      </c>
-      <c r="J66" s="0" t="n">
-        <v>6.82834475297512</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="B67" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>50</v>
+        <v>81</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>221</v>
       </c>
-      <c r="E67" s="1" t="n">
+      <c r="E67" s="2" t="n">
         <v>221</v>
       </c>
-      <c r="H67" s="0" t="s">
-        <v>17</v>
+      <c r="F67" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B68" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>50</v>
+        <v>82</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D68" s="0" t="n">
         <v>221</v>
       </c>
-      <c r="E68" s="1" t="n">
+      <c r="E68" s="2" t="n">
         <v>221</v>
       </c>
-      <c r="H68" s="0" t="s">
-        <v>17</v>
+      <c r="F68" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="B69" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>50</v>
+        <v>83</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>221</v>
       </c>
-      <c r="E69" s="1" t="n">
+      <c r="E69" s="2" t="n">
         <v>221</v>
       </c>
-      <c r="H69" s="0" t="s">
-        <v>17</v>
+      <c r="F69" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B70" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>50</v>
+        <v>84</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>221</v>
       </c>
-      <c r="E70" s="1" t="n">
+      <c r="E70" s="2" t="n">
         <v>221</v>
       </c>
-      <c r="H70" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I70" s="0" t="n">
-        <v>8.99420819996952</v>
-      </c>
-      <c r="J70" s="0" t="n">
+      <c r="F70" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H70" s="0" t="n">
         <v>8.58108995403808</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="B71" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>50</v>
+        <v>85</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D71" s="0" t="n">
         <v>586</v>
       </c>
-      <c r="E71" s="1" t="n">
+      <c r="E71" s="2" t="n">
         <v>586</v>
       </c>
-      <c r="F71" s="0" t="n">
+      <c r="F71" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G71" s="0" t="n">
         <v>5.35131205</v>
       </c>
-      <c r="G71" s="0" t="n">
+      <c r="H71" s="0" t="n">
+        <v>6.19074177356386</v>
+      </c>
+      <c r="I71" s="0" t="n">
         <v>54.4451539</v>
-      </c>
-      <c r="H71" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I71" s="0" t="n">
-        <v>6.30870495310186</v>
-      </c>
-      <c r="J71" s="0" t="n">
-        <v>6.19074177356386</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="B72" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>50</v>
+        <v>86</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>586</v>
       </c>
-      <c r="E72" s="1" t="n">
+      <c r="E72" s="2" t="n">
         <v>586</v>
       </c>
-      <c r="H72" s="0" t="s">
-        <v>17</v>
+      <c r="F72" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="B73" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C73" s="0" t="s">
-        <v>50</v>
+        <v>87</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>586</v>
       </c>
-      <c r="E73" s="1" t="n">
+      <c r="E73" s="2" t="n">
         <v>586</v>
       </c>
-      <c r="H73" s="0" t="s">
-        <v>17</v>
+      <c r="F73" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="B74" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>50</v>
+        <v>88</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C74" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>586</v>
       </c>
-      <c r="E74" s="1" t="n">
+      <c r="E74" s="2" t="n">
         <v>586</v>
       </c>
-      <c r="H74" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I74" s="0" t="n">
-        <v>8.65703651187522</v>
-      </c>
-      <c r="J74" s="0" t="n">
+      <c r="F74" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H74" s="0" t="n">
         <v>9.13349633251834</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B75" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C75" s="0" t="s">
-        <v>50</v>
+        <v>89</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C75" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D75" s="0" t="n">
         <v>586</v>
       </c>
-      <c r="E75" s="1" t="n">
+      <c r="E75" s="2" t="n">
         <v>586</v>
       </c>
-      <c r="H75" s="0" t="s">
-        <v>17</v>
+      <c r="F75" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="B76" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>50</v>
+        <v>90</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>145</v>
       </c>
-      <c r="E76" s="1" t="n">
+      <c r="E76" s="2" t="n">
         <v>145</v>
       </c>
-      <c r="F76" s="0" t="n">
+      <c r="F76" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G76" s="0" t="n">
         <v>16.09712027</v>
       </c>
-      <c r="G76" s="0" t="n">
+      <c r="H76" s="0" t="n">
+        <v>6.04868549172347</v>
+      </c>
+      <c r="I76" s="0" t="n">
         <v>20.25935053</v>
-      </c>
-      <c r="H76" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I76" s="0" t="n">
-        <v>10.9454828660436</v>
-      </c>
-      <c r="J76" s="0" t="n">
-        <v>6.04868549172347</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="B77" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>50</v>
+        <v>91</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D77" s="0" t="n">
         <v>145</v>
       </c>
-      <c r="E77" s="1" t="n">
+      <c r="E77" s="2" t="n">
         <v>145</v>
       </c>
-      <c r="H77" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I77" s="0" t="n">
-        <v>9.29873853211009</v>
-      </c>
-      <c r="J77" s="0" t="n">
+      <c r="F77" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H77" s="0" t="n">
         <v>8.32882462686567</v>
+      </c>
+      <c r="L77" s="0" t="n">
+        <v>181</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="B78" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>50</v>
+        <v>92</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D78" s="0" t="n">
         <v>145</v>
       </c>
-      <c r="E78" s="1" t="n">
+      <c r="E78" s="2" t="n">
         <v>145</v>
       </c>
-      <c r="H78" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I78" s="0" t="n">
-        <v>19.199203187251</v>
-      </c>
-      <c r="J78" s="0" t="n">
+      <c r="F78" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H78" s="0" t="n">
         <v>12.3678756476684</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="B79" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>50</v>
+        <v>93</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D79" s="0" t="n">
         <v>288</v>
       </c>
-      <c r="E79" s="1" t="n">
+      <c r="E79" s="2" t="n">
         <v>288</v>
       </c>
-      <c r="F79" s="0" t="n">
+      <c r="F79" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G79" s="0" t="n">
         <v>9.216589862</v>
       </c>
-      <c r="G79" s="0" t="n">
+      <c r="H79" s="0" t="n">
+        <v>7.42969396195203</v>
+      </c>
+      <c r="I79" s="0" t="n">
         <v>113.4440422</v>
-      </c>
-      <c r="H79" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I79" s="0" t="n">
-        <v>8.73694779116466</v>
-      </c>
-      <c r="J79" s="0" t="n">
-        <v>7.42969396195203</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="B80" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>50</v>
+        <v>94</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D80" s="0" t="n">
         <v>93</v>
       </c>
-      <c r="E80" s="1" t="n">
+      <c r="E80" s="2" t="n">
         <v>93</v>
       </c>
-      <c r="F80" s="0" t="n">
+      <c r="F80" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G80" s="0" t="n">
         <v>13.12777285</v>
       </c>
-      <c r="G80" s="0" t="n">
+      <c r="H80" s="0" t="n">
+        <v>9.40529531568228</v>
+      </c>
+      <c r="I80" s="0" t="n">
         <v>29.19970064</v>
-      </c>
-      <c r="H80" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I80" s="0" t="n">
-        <v>11.350332594235</v>
-      </c>
-      <c r="J80" s="0" t="n">
-        <v>9.40529531568228</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="B81" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C81" s="0" t="s">
-        <v>50</v>
+        <v>95</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D81" s="0" t="n">
         <v>93</v>
       </c>
-      <c r="E81" s="1" t="n">
+      <c r="E81" s="2" t="n">
         <v>93</v>
       </c>
-      <c r="H81" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I81" s="0" t="n">
-        <v>5.93717524799244</v>
-      </c>
-      <c r="J81" s="0" t="n">
+      <c r="F81" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H81" s="0" t="n">
         <v>8.89652777777778</v>
+      </c>
+      <c r="L81" s="0" t="n">
+        <v>160</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="B82" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>50</v>
+        <v>96</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>93</v>
       </c>
-      <c r="E82" s="1" t="n">
+      <c r="E82" s="2" t="n">
         <v>93</v>
       </c>
-      <c r="H82" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I82" s="0" t="n">
-        <v>18.6184738955823</v>
-      </c>
-      <c r="J82" s="0" t="n">
+      <c r="F82" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H82" s="0" t="n">
         <v>10.8880952380952</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="B83" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>50</v>
+        <v>97</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D83" s="0" t="n">
         <v>143</v>
       </c>
-      <c r="E83" s="1" t="n">
+      <c r="E83" s="2" t="n">
         <v>143</v>
       </c>
-      <c r="F83" s="0" t="n">
+      <c r="F83" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G83" s="0" t="n">
         <v>54.63414634</v>
       </c>
-      <c r="G83" s="0" t="n">
+      <c r="H83" s="0" t="n">
+        <v>12.2922794117647</v>
+      </c>
+      <c r="I83" s="0" t="n">
         <v>44.60837344</v>
-      </c>
-      <c r="H83" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I83" s="0" t="n">
-        <v>12.1381118881119</v>
-      </c>
-      <c r="J83" s="0" t="n">
-        <v>12.2922794117647</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="B84" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>50</v>
+        <v>98</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D84" s="0" t="n">
         <v>143</v>
       </c>
-      <c r="E84" s="1" t="n">
+      <c r="E84" s="2" t="n">
         <v>143</v>
       </c>
-      <c r="H84" s="0" t="s">
-        <v>17</v>
+      <c r="F84" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B85" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C85" s="0" t="s">
-        <v>50</v>
+        <v>99</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C85" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D85" s="0" t="n">
         <v>143</v>
       </c>
-      <c r="E85" s="1" t="n">
+      <c r="E85" s="2" t="n">
         <v>143</v>
       </c>
-      <c r="H85" s="0" t="s">
-        <v>17</v>
+      <c r="F85" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B86" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>50</v>
+        <v>100</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C86" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D86" s="0" t="n">
         <v>143</v>
       </c>
-      <c r="E86" s="1" t="n">
+      <c r="E86" s="2" t="n">
         <v>143</v>
       </c>
-      <c r="H86" s="0" t="s">
-        <v>17</v>
+      <c r="F86" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B87" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C87" s="0" t="s">
-        <v>50</v>
+        <v>101</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C87" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D87" s="0" t="n">
         <v>143</v>
       </c>
-      <c r="E87" s="1" t="n">
+      <c r="E87" s="2" t="n">
         <v>143</v>
       </c>
-      <c r="H87" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I87" s="0" t="n">
-        <v>8.8652870764861</v>
-      </c>
-      <c r="J87" s="0" t="n">
+      <c r="F87" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H87" s="0" t="n">
         <v>8.09428794992175</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B88" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>50</v>
+        <v>102</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C88" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D88" s="0" t="n">
         <v>143</v>
       </c>
-      <c r="E88" s="1" t="n">
+      <c r="E88" s="2" t="n">
         <v>143</v>
       </c>
-      <c r="H88" s="0" t="s">
-        <v>17</v>
+      <c r="F88" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="B89" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C89" s="0" t="s">
-        <v>50</v>
+        <v>103</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C89" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D89" s="0" t="n">
         <v>843</v>
       </c>
-      <c r="E89" s="1" t="n">
+      <c r="E89" s="2" t="n">
         <v>843</v>
       </c>
-      <c r="G89" s="0" t="n">
+      <c r="F89" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H89" s="0" t="n">
+        <v>4.51894411621226</v>
+      </c>
+      <c r="I89" s="0" t="n">
         <v>28.51596639</v>
-      </c>
-      <c r="H89" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I89" s="0" t="n">
-        <v>4.53683451508232</v>
-      </c>
-      <c r="J89" s="0" t="n">
-        <v>4.51894411621226</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="B90" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C90" s="0" t="s">
-        <v>50</v>
+        <v>104</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C90" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D90" s="0" t="n">
         <v>843</v>
       </c>
-      <c r="E90" s="1" t="n">
+      <c r="E90" s="2" t="n">
         <v>843</v>
       </c>
-      <c r="H90" s="0" t="s">
-        <v>17</v>
+      <c r="F90" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="B91" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C91" s="0" t="s">
-        <v>50</v>
+        <v>105</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C91" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D91" s="0" t="n">
         <v>843</v>
       </c>
-      <c r="E91" s="1" t="n">
+      <c r="E91" s="2" t="n">
         <v>843</v>
       </c>
-      <c r="H91" s="0" t="s">
-        <v>17</v>
+      <c r="F91" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B92" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C92" s="0" t="s">
-        <v>50</v>
+        <v>106</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C92" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D92" s="0" t="n">
         <v>843</v>
       </c>
-      <c r="E92" s="1" t="n">
+      <c r="E92" s="2" t="n">
         <v>843</v>
       </c>
-      <c r="H92" s="0" t="s">
-        <v>17</v>
+      <c r="F92" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B93" s="0" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C93" s="0" t="s">
-        <v>50</v>
+        <v>107</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C93" s="0" t="n">
+        <v>2018</v>
       </c>
       <c r="D93" s="0" t="n">
         <v>843</v>
       </c>
-      <c r="E93" s="1" t="n">
+      <c r="E93" s="2" t="n">
         <v>843</v>
       </c>
-      <c r="H93" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I93" s="0" t="n">
-        <v>9.16191030867793</v>
-      </c>
-      <c r="J93" s="0" t="n">
+      <c r="F93" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H93" s="0" t="n">
         <v>8.58502772643253</v>
       </c>
     </row>
@@ -4440,25 +4335,25 @@
       <selection pane="topLeft" activeCell="T38" activeCellId="0" sqref="T38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>50</v>
@@ -4473,7 +4368,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>93</v>
@@ -4488,7 +4383,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>120</v>
@@ -4503,7 +4398,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>122</v>
@@ -4518,7 +4413,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>143</v>
@@ -4533,7 +4428,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>145</v>
@@ -4548,7 +4443,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>190</v>
@@ -4563,7 +4458,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>201</v>
@@ -4578,7 +4473,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>221</v>
@@ -4593,7 +4488,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>288</v>
@@ -4608,7 +4503,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>586</v>
@@ -4623,7 +4518,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>843</v>
@@ -4638,21 +4533,21 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>85</v>
@@ -4667,7 +4562,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>87</v>
@@ -4682,7 +4577,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>121</v>
@@ -4697,7 +4592,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>147</v>
@@ -4712,7 +4607,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>151</v>
@@ -4727,7 +4622,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>368</v>
@@ -4742,7 +4637,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>586</v>

</xml_diff>

<commit_message>
plotted adjusted n2 rates from 2017 and 2018 in python new nb
</commit_message>
<xml_diff>
--- a/data/flux/2018-fluxes.xlsx
+++ b/data/flux/2018-fluxes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="113">
   <si>
     <t xml:space="preserve">sample id</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t xml:space="preserve">N production rate (nM N/day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adjusted N prod (nM N/day)</t>
   </si>
   <si>
     <t xml:space="preserve">1-30_151m_+P</t>
@@ -532,7 +535,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart109.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -733,11 +736,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="42389324"/>
-        <c:axId val="25263661"/>
+        <c:axId val="35953532"/>
+        <c:axId val="47663203"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42389324"/>
+        <c:axId val="35953532"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -793,12 +796,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25263661"/>
+        <c:crossAx val="47663203"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="25263661"/>
+        <c:axId val="47663203"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -863,7 +866,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42389324"/>
+        <c:crossAx val="35953532"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -911,7 +914,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart110.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1082,11 +1085,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="4628659"/>
-        <c:axId val="62961195"/>
+        <c:axId val="81976547"/>
+        <c:axId val="19695846"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="4628659"/>
+        <c:axId val="81976547"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1142,12 +1145,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62961195"/>
+        <c:crossAx val="19695846"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62961195"/>
+        <c:axId val="19695846"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1212,7 +1215,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4628659"/>
+        <c:crossAx val="81976547"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1260,7 +1263,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart111.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1461,11 +1464,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="34787098"/>
-        <c:axId val="55617147"/>
+        <c:axId val="23514814"/>
+        <c:axId val="11888493"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="34787098"/>
+        <c:axId val="23514814"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1521,12 +1524,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55617147"/>
+        <c:crossAx val="11888493"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55617147"/>
+        <c:axId val="11888493"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1591,7 +1594,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34787098"/>
+        <c:crossAx val="23514814"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1639,7 +1642,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart112.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1810,11 +1813,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="16626035"/>
-        <c:axId val="66205091"/>
+        <c:axId val="97330228"/>
+        <c:axId val="64868907"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="16626035"/>
+        <c:axId val="97330228"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1870,12 +1873,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66205091"/>
+        <c:crossAx val="64868907"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66205091"/>
+        <c:axId val="64868907"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1940,7 +1943,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16626035"/>
+        <c:crossAx val="97330228"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1999,9 +2002,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>718920</xdr:colOff>
+      <xdr:colOff>718560</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2009,8 +2012,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5073120" y="86040"/>
-        <a:ext cx="5445000" cy="4550400"/>
+        <a:off x="5080680" y="86040"/>
+        <a:ext cx="5452200" cy="4550040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2029,9 +2032,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>225360</xdr:colOff>
+      <xdr:colOff>225000</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2039,8 +2042,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5066280" y="4924800"/>
-        <a:ext cx="4958280" cy="4722480"/>
+        <a:off x="5073840" y="4924800"/>
+        <a:ext cx="4965480" cy="4722120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2059,9 +2062,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>605160</xdr:colOff>
+      <xdr:colOff>604800</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2069,8 +2072,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10675440" y="0"/>
-        <a:ext cx="5445000" cy="4550400"/>
+        <a:off x="10692000" y="0"/>
+        <a:ext cx="5452200" cy="4550040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2089,9 +2092,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>98640</xdr:colOff>
+      <xdr:colOff>98280</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>104400</xdr:rowOff>
+      <xdr:rowOff>104040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2099,8 +2102,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10655640" y="4972680"/>
-        <a:ext cx="4958280" cy="4722480"/>
+        <a:off x="10672200" y="4972680"/>
+        <a:ext cx="4965480" cy="4722120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2118,13 +2121,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L93"/>
+  <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.26"/>
@@ -2175,13 +2178,16 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>2018</v>
@@ -2193,7 +2199,7 @@
         <v>151</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>59.93179319</v>
@@ -2207,13 +2213,16 @@
       <c r="L2" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="M2" s="0" t="n">
+        <v>0.22</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>2018</v>
@@ -2225,7 +2234,7 @@
         <v>151</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>58.1495726495727</v>
@@ -2233,10 +2242,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2018</v>
@@ -2248,7 +2257,7 @@
         <v>121</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>140.2346446</v>
@@ -2262,10 +2271,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>2018</v>
@@ -2277,7 +2286,7 @@
         <v>121</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>76.4009433962264</v>
@@ -2285,10 +2294,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>2018</v>
@@ -2300,15 +2309,15 @@
         <v>147</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>2018</v>
@@ -2320,7 +2329,7 @@
         <v>147</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>135.5691057</v>
@@ -2331,10 +2340,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>2018</v>
@@ -2346,15 +2355,15 @@
         <v>147</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>2018</v>
@@ -2366,7 +2375,7 @@
         <v>147</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>20.0629370629371</v>
@@ -2374,10 +2383,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>2018</v>
@@ -2389,7 +2398,7 @@
         <v>147</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>9.29615547106041</v>
@@ -2397,10 +2406,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>2018</v>
@@ -2412,15 +2421,15 @@
         <v>147</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>2018</v>
@@ -2432,15 +2441,15 @@
         <v>147</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>2018</v>
@@ -2452,15 +2461,15 @@
         <v>147</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>2018</v>
@@ -2472,7 +2481,7 @@
         <v>368</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>5.577733349</v>
@@ -2486,10 +2495,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>2018</v>
@@ -2501,7 +2510,7 @@
         <v>368</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>7.78433862433862</v>
@@ -2509,13 +2518,16 @@
       <c r="L15" s="0" t="n">
         <v>375</v>
       </c>
+      <c r="M15" s="0" t="n">
+        <v>12.09</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>2018</v>
@@ -2527,7 +2539,7 @@
         <v>368</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>31.2538461538462</v>
@@ -2535,10 +2547,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>2018</v>
@@ -2550,15 +2562,15 @@
         <v>368</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>2018</v>
@@ -2570,15 +2582,15 @@
         <v>368</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>2018</v>
@@ -2590,7 +2602,7 @@
         <v>368</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>7.1683748169839</v>
@@ -2598,10 +2610,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>2018</v>
@@ -2613,7 +2625,7 @@
         <v>586</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>8.164440297</v>
@@ -2627,10 +2639,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>2018</v>
@@ -2642,7 +2654,7 @@
         <v>586</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>7.24497117232543</v>
@@ -2650,10 +2662,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>2018</v>
@@ -2665,15 +2677,15 @@
         <v>586</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>2018</v>
@@ -2685,7 +2697,7 @@
         <v>586</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H23" s="0" t="n">
         <v>10.5844394527262</v>
@@ -2693,10 +2705,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>2018</v>
@@ -2708,7 +2720,7 @@
         <v>87</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G24" s="0" t="n">
         <v>24.18012422</v>
@@ -2722,10 +2734,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>2018</v>
@@ -2737,7 +2749,7 @@
         <v>87</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H25" s="0" t="n">
         <v>4.95272525027809</v>
@@ -2745,13 +2757,16 @@
       <c r="L25" s="0" t="n">
         <v>38.5</v>
       </c>
+      <c r="M25" s="0" t="n">
+        <v>7.32</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>2018</v>
@@ -2763,7 +2778,7 @@
         <v>87</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>10.8071895424837</v>
@@ -2771,10 +2786,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>2018</v>
@@ -2786,7 +2801,7 @@
         <v>221</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H27" s="0" t="n">
         <v>11.6933911159263</v>
@@ -2794,10 +2809,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>2018</v>
@@ -2809,7 +2824,7 @@
         <v>221</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H28" s="0" t="n">
         <v>2.63057324840764</v>
@@ -2817,13 +2832,16 @@
       <c r="L28" s="0" t="n">
         <v>13</v>
       </c>
+      <c r="M28" s="0" t="n">
+        <v>18.46</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>2018</v>
@@ -2835,7 +2853,7 @@
         <v>221</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H29" s="0" t="n">
         <v>5.58258642765685</v>
@@ -2843,10 +2861,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>2018</v>
@@ -2858,7 +2876,7 @@
         <v>85</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G30" s="0" t="n">
         <v>26.58868425</v>
@@ -2872,10 +2890,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>2018</v>
@@ -2887,7 +2905,7 @@
         <v>85</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H31" s="0" t="n">
         <v>5.66409124356144</v>
@@ -2895,13 +2913,16 @@
       <c r="L31" s="0" t="n">
         <v>530</v>
       </c>
+      <c r="M31" s="0" t="n">
+        <v>21.09</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>2018</v>
@@ -2913,7 +2934,7 @@
         <v>85</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>13.2683760683761</v>
@@ -2921,10 +2942,10 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>2018</v>
@@ -2936,15 +2957,15 @@
         <v>85</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>2018</v>
@@ -2956,7 +2977,7 @@
         <v>85</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H34" s="0" t="n">
         <v>8.43557336621455</v>
@@ -2964,10 +2985,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>2018</v>
@@ -2979,15 +3000,15 @@
         <v>85</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>2018</v>
@@ -2999,7 +3020,7 @@
         <v>147</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H36" s="0" t="n">
         <v>6.97915798249271</v>
@@ -3007,10 +3028,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>2018</v>
@@ -3022,15 +3043,15 @@
         <v>147</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>2018</v>
@@ -3042,7 +3063,7 @@
         <v>50</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H38" s="0" t="n">
         <v>6.7035458711908</v>
@@ -3053,10 +3074,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>2018</v>
@@ -3068,15 +3089,15 @@
         <v>50</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>2018</v>
@@ -3088,15 +3109,15 @@
         <v>50</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>2018</v>
@@ -3108,7 +3129,7 @@
         <v>50</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H41" s="0" t="n">
         <v>7.96274373259053</v>
@@ -3116,10 +3137,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>2018</v>
@@ -3131,7 +3152,7 @@
         <v>120</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H42" s="0" t="n">
         <v>6.35134728285413</v>
@@ -3139,10 +3160,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>2018</v>
@@ -3154,15 +3175,15 @@
         <v>120</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>2018</v>
@@ -3174,15 +3195,15 @@
         <v>120</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>2018</v>
@@ -3194,7 +3215,7 @@
         <v>120</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H45" s="0" t="n">
         <v>7.10068803490519</v>
@@ -3202,10 +3223,10 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>2018</v>
@@ -3217,15 +3238,15 @@
         <v>120</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>2018</v>
@@ -3237,7 +3258,7 @@
         <v>122</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G47" s="0" t="n">
         <v>32.66219522</v>
@@ -3251,10 +3272,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>2018</v>
@@ -3266,7 +3287,7 @@
         <v>122</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H48" s="0" t="n">
         <v>2.96830864622804</v>
@@ -3274,13 +3295,16 @@
       <c r="L48" s="0" t="n">
         <v>54</v>
       </c>
+      <c r="M48" s="0" t="n">
+        <v>9.88</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>2018</v>
@@ -3292,7 +3316,7 @@
         <v>122</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H49" s="0" t="n">
         <v>9.47640449438202</v>
@@ -3300,10 +3324,10 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>2018</v>
@@ -3315,7 +3339,7 @@
         <v>120</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G50" s="0" t="n">
         <v>144.5962733</v>
@@ -3326,10 +3350,10 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>2018</v>
@@ -3341,7 +3365,7 @@
         <v>190</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G51" s="0" t="n">
         <v>31.86596927</v>
@@ -3355,10 +3379,10 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>2018</v>
@@ -3370,7 +3394,7 @@
         <v>190</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H52" s="0" t="n">
         <v>4.91321499013807</v>
@@ -3378,13 +3402,16 @@
       <c r="L52" s="0" t="n">
         <v>64</v>
       </c>
+      <c r="M52" s="0" t="n">
+        <v>6.97</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C53" s="0" t="n">
         <v>2018</v>
@@ -3396,7 +3423,7 @@
         <v>190</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H53" s="0" t="n">
         <v>2.77491749174917</v>
@@ -3404,10 +3431,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C54" s="0" t="n">
         <v>2018</v>
@@ -3419,7 +3446,7 @@
         <v>123</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G54" s="0" t="n">
         <v>127.6422764</v>
@@ -3427,10 +3454,10 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>2018</v>
@@ -3442,15 +3469,15 @@
         <v>123</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>2018</v>
@@ -3462,15 +3489,15 @@
         <v>123</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C57" s="0" t="n">
         <v>2018</v>
@@ -3482,7 +3509,7 @@
         <v>123</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H57" s="0" t="n">
         <v>8.21664180341455</v>
@@ -3490,10 +3517,10 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C58" s="0" t="n">
         <v>2018</v>
@@ -3505,7 +3532,7 @@
         <v>201</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G58" s="0" t="n">
         <v>18.53988134</v>
@@ -3519,10 +3546,10 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C59" s="0" t="n">
         <v>2018</v>
@@ -3534,7 +3561,7 @@
         <v>201</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H59" s="0" t="n">
         <v>13.01269035533</v>
@@ -3542,10 +3569,10 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C60" s="0" t="n">
         <v>2018</v>
@@ -3557,7 +3584,7 @@
         <v>201</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H60" s="0" t="n">
         <v>8.47593418422267</v>
@@ -3565,10 +3592,10 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C61" s="0" t="n">
         <v>2018</v>
@@ -3580,15 +3607,15 @@
         <v>201</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C62" s="0" t="n">
         <v>2018</v>
@@ -3600,15 +3627,15 @@
         <v>201</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C63" s="0" t="n">
         <v>2018</v>
@@ -3620,15 +3647,15 @@
         <v>201</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C64" s="0" t="n">
         <v>2018</v>
@@ -3640,15 +3667,15 @@
         <v>201</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C65" s="0" t="n">
         <v>2018</v>
@@ -3660,15 +3687,15 @@
         <v>221</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C66" s="0" t="n">
         <v>2018</v>
@@ -3680,7 +3707,7 @@
         <v>221</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G66" s="0" t="n">
         <v>7.360697997</v>
@@ -3694,10 +3721,10 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C67" s="0" t="n">
         <v>2018</v>
@@ -3709,15 +3736,15 @@
         <v>221</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C68" s="0" t="n">
         <v>2018</v>
@@ -3729,15 +3756,15 @@
         <v>221</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C69" s="0" t="n">
         <v>2018</v>
@@ -3749,15 +3776,15 @@
         <v>221</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C70" s="0" t="n">
         <v>2018</v>
@@ -3769,7 +3796,7 @@
         <v>221</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H70" s="0" t="n">
         <v>8.58108995403808</v>
@@ -3777,10 +3804,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C71" s="0" t="n">
         <v>2018</v>
@@ -3792,7 +3819,7 @@
         <v>586</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G71" s="0" t="n">
         <v>5.35131205</v>
@@ -3806,10 +3833,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C72" s="0" t="n">
         <v>2018</v>
@@ -3821,15 +3848,15 @@
         <v>586</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C73" s="0" t="n">
         <v>2018</v>
@@ -3841,15 +3868,15 @@
         <v>586</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C74" s="0" t="n">
         <v>2018</v>
@@ -3861,7 +3888,7 @@
         <v>586</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H74" s="0" t="n">
         <v>9.13349633251834</v>
@@ -3869,10 +3896,10 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C75" s="0" t="n">
         <v>2018</v>
@@ -3884,15 +3911,15 @@
         <v>586</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C76" s="0" t="n">
         <v>2018</v>
@@ -3904,7 +3931,7 @@
         <v>145</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G76" s="0" t="n">
         <v>16.09712027</v>
@@ -3918,10 +3945,10 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C77" s="0" t="n">
         <v>2018</v>
@@ -3933,7 +3960,7 @@
         <v>145</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H77" s="0" t="n">
         <v>8.32882462686567</v>
@@ -3941,13 +3968,16 @@
       <c r="L77" s="0" t="n">
         <v>181</v>
       </c>
+      <c r="M77" s="0" t="n">
+        <v>7.36</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C78" s="0" t="n">
         <v>2018</v>
@@ -3959,7 +3989,7 @@
         <v>145</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H78" s="0" t="n">
         <v>12.3678756476684</v>
@@ -3967,10 +3997,10 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C79" s="0" t="n">
         <v>2018</v>
@@ -3982,7 +4012,7 @@
         <v>288</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G79" s="0" t="n">
         <v>9.216589862</v>
@@ -3996,10 +4026,10 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C80" s="0" t="n">
         <v>2018</v>
@@ -4011,7 +4041,7 @@
         <v>93</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G80" s="0" t="n">
         <v>13.12777285</v>
@@ -4025,10 +4055,10 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C81" s="0" t="n">
         <v>2018</v>
@@ -4040,7 +4070,7 @@
         <v>93</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H81" s="0" t="n">
         <v>8.89652777777778</v>
@@ -4048,13 +4078,16 @@
       <c r="L81" s="0" t="n">
         <v>160</v>
       </c>
+      <c r="M81" s="0" t="n">
+        <v>12.96</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C82" s="0" t="n">
         <v>2018</v>
@@ -4066,7 +4099,7 @@
         <v>93</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H82" s="0" t="n">
         <v>10.8880952380952</v>
@@ -4074,10 +4107,10 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C83" s="0" t="n">
         <v>2018</v>
@@ -4089,7 +4122,7 @@
         <v>143</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G83" s="0" t="n">
         <v>54.63414634</v>
@@ -4103,10 +4136,10 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C84" s="0" t="n">
         <v>2018</v>
@@ -4118,15 +4151,15 @@
         <v>143</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C85" s="0" t="n">
         <v>2018</v>
@@ -4138,15 +4171,15 @@
         <v>143</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C86" s="0" t="n">
         <v>2018</v>
@@ -4158,15 +4191,15 @@
         <v>143</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C87" s="0" t="n">
         <v>2018</v>
@@ -4178,7 +4211,7 @@
         <v>143</v>
       </c>
       <c r="F87" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H87" s="0" t="n">
         <v>8.09428794992175</v>
@@ -4186,10 +4219,10 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C88" s="0" t="n">
         <v>2018</v>
@@ -4201,15 +4234,15 @@
         <v>143</v>
       </c>
       <c r="F88" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C89" s="0" t="n">
         <v>2018</v>
@@ -4221,7 +4254,7 @@
         <v>843</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H89" s="0" t="n">
         <v>4.51894411621226</v>
@@ -4232,10 +4265,10 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C90" s="0" t="n">
         <v>2018</v>
@@ -4247,15 +4280,15 @@
         <v>843</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C91" s="0" t="n">
         <v>2018</v>
@@ -4267,15 +4300,15 @@
         <v>843</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C92" s="0" t="n">
         <v>2018</v>
@@ -4287,15 +4320,15 @@
         <v>843</v>
       </c>
       <c r="F92" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C93" s="0" t="n">
         <v>2018</v>
@@ -4307,7 +4340,7 @@
         <v>843</v>
       </c>
       <c r="F93" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H93" s="0" t="n">
         <v>8.58502772643253</v>
@@ -4335,25 +4368,25 @@
       <selection pane="topLeft" activeCell="T38" activeCellId="0" sqref="T38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>50</v>
@@ -4368,7 +4401,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>93</v>
@@ -4383,7 +4416,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>120</v>
@@ -4398,7 +4431,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>122</v>
@@ -4413,7 +4446,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>143</v>
@@ -4428,7 +4461,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>145</v>
@@ -4443,7 +4476,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>190</v>
@@ -4458,7 +4491,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>201</v>
@@ -4473,7 +4506,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>221</v>
@@ -4488,7 +4521,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>288</v>
@@ -4503,7 +4536,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>586</v>
@@ -4518,7 +4551,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>843</v>
@@ -4536,18 +4569,18 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>85</v>
@@ -4562,7 +4595,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>87</v>
@@ -4577,7 +4610,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>121</v>
@@ -4592,7 +4625,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>147</v>
@@ -4607,7 +4640,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>151</v>
@@ -4622,7 +4655,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>368</v>
@@ -4637,7 +4670,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>586</v>

</xml_diff>

<commit_message>
made lines for anoxia on rate plots
</commit_message>
<xml_diff>
--- a/data/flux/2018-fluxes.xlsx
+++ b/data/flux/2018-fluxes.xlsx
@@ -535,7 +535,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart109.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart113.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -736,11 +736,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="35953532"/>
-        <c:axId val="47663203"/>
+        <c:axId val="95005120"/>
+        <c:axId val="3301010"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="35953532"/>
+        <c:axId val="95005120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -796,12 +796,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47663203"/>
+        <c:crossAx val="3301010"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47663203"/>
+        <c:axId val="3301010"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -866,7 +866,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35953532"/>
+        <c:crossAx val="95005120"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -914,7 +914,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart110.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart114.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1085,11 +1085,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="81976547"/>
-        <c:axId val="19695846"/>
+        <c:axId val="21512473"/>
+        <c:axId val="58273497"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81976547"/>
+        <c:axId val="21512473"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1145,12 +1145,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19695846"/>
+        <c:crossAx val="58273497"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="19695846"/>
+        <c:axId val="58273497"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1215,7 +1215,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81976547"/>
+        <c:crossAx val="21512473"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1263,7 +1263,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart111.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart115.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1464,11 +1464,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="23514814"/>
-        <c:axId val="11888493"/>
+        <c:axId val="67952650"/>
+        <c:axId val="53403612"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="23514814"/>
+        <c:axId val="67952650"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1524,12 +1524,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11888493"/>
+        <c:crossAx val="53403612"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="11888493"/>
+        <c:axId val="53403612"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1594,7 +1594,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23514814"/>
+        <c:crossAx val="67952650"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1642,7 +1642,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart112.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart116.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1813,11 +1813,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="97330228"/>
-        <c:axId val="64868907"/>
+        <c:axId val="62324970"/>
+        <c:axId val="27608640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97330228"/>
+        <c:axId val="62324970"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1873,12 +1873,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64868907"/>
+        <c:crossAx val="27608640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64868907"/>
+        <c:axId val="27608640"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1943,7 +1943,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97330228"/>
+        <c:crossAx val="62324970"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2124,7 +2124,7 @@
   <dimension ref="A1:M93"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
+      <selection pane="topLeft" activeCell="M31" activeCellId="0" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
added babbin rates to plots
</commit_message>
<xml_diff>
--- a/data/flux/2018-fluxes.xlsx
+++ b/data/flux/2018-fluxes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="114">
   <si>
     <t xml:space="preserve">sample id</t>
   </si>
@@ -62,12 +62,18 @@
     <t xml:space="preserve">Adjusted N prod (nM N/day)</t>
   </si>
   <si>
+    <t xml:space="preserve">Babbin N production rates  (nM N/day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">net</t>
+  </si>
+  <si>
     <t xml:space="preserve">1-30_151m_+P</t>
   </si>
   <si>
-    <t xml:space="preserve">P2</t>
-  </si>
-  <si>
     <t xml:space="preserve">cone</t>
   </si>
   <si>
@@ -81,9 +87,6 @@
   </si>
   <si>
     <t xml:space="preserve">3-32_147m_top_remainder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">net</t>
   </si>
   <si>
     <t xml:space="preserve">3-32_147m_top</t>
@@ -535,7 +538,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart113.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart131.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -736,11 +739,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="95005120"/>
-        <c:axId val="3301010"/>
+        <c:axId val="36488341"/>
+        <c:axId val="868967"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95005120"/>
+        <c:axId val="36488341"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -796,12 +799,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3301010"/>
+        <c:crossAx val="868967"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="3301010"/>
+        <c:axId val="868967"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -866,7 +869,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95005120"/>
+        <c:crossAx val="36488341"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -914,7 +917,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart114.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart132.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1085,11 +1088,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="21512473"/>
-        <c:axId val="58273497"/>
+        <c:axId val="88112210"/>
+        <c:axId val="36782191"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="21512473"/>
+        <c:axId val="88112210"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1145,12 +1148,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58273497"/>
+        <c:crossAx val="36782191"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58273497"/>
+        <c:axId val="36782191"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1215,7 +1218,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21512473"/>
+        <c:crossAx val="88112210"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1263,7 +1266,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart115.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart133.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1464,11 +1467,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="67952650"/>
-        <c:axId val="53403612"/>
+        <c:axId val="31688535"/>
+        <c:axId val="10576364"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67952650"/>
+        <c:axId val="31688535"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1524,12 +1527,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53403612"/>
+        <c:crossAx val="10576364"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53403612"/>
+        <c:axId val="10576364"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1594,7 +1597,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67952650"/>
+        <c:crossAx val="31688535"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1642,7 +1645,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart116.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart134.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1813,11 +1816,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="62324970"/>
-        <c:axId val="27608640"/>
+        <c:axId val="7497611"/>
+        <c:axId val="18671237"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="62324970"/>
+        <c:axId val="7497611"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1873,12 +1876,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27608640"/>
+        <c:crossAx val="18671237"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="27608640"/>
+        <c:axId val="18671237"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1943,7 +1946,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62324970"/>
+        <c:crossAx val="7497611"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2002,9 +2005,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>718560</xdr:colOff>
+      <xdr:colOff>718200</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>84600</xdr:rowOff>
+      <xdr:rowOff>84240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2012,8 +2015,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5080680" y="86040"/>
-        <a:ext cx="5452200" cy="4550040"/>
+        <a:off x="5088240" y="86040"/>
+        <a:ext cx="5459760" cy="4549680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2032,9 +2035,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>225000</xdr:colOff>
+      <xdr:colOff>224640</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>56160</xdr:rowOff>
+      <xdr:rowOff>55800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2042,8 +2045,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5073840" y="4924800"/>
-        <a:ext cx="4965480" cy="4722120"/>
+        <a:off x="5081400" y="4924800"/>
+        <a:ext cx="4973040" cy="4721760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2062,9 +2065,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>604800</xdr:colOff>
+      <xdr:colOff>604440</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>160920</xdr:rowOff>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2072,8 +2075,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10692000" y="0"/>
-        <a:ext cx="5452200" cy="4550040"/>
+        <a:off x="10708560" y="0"/>
+        <a:ext cx="5459400" cy="4549680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2092,9 +2095,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>98280</xdr:colOff>
+      <xdr:colOff>97920</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>104040</xdr:rowOff>
+      <xdr:rowOff>103680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2102,8 +2105,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10672200" y="4972680"/>
-        <a:ext cx="4965480" cy="4722120"/>
+        <a:off x="10688760" y="4972680"/>
+        <a:ext cx="4972680" cy="4721760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2121,13 +2124,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M93"/>
+  <dimension ref="A1:N96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M31" activeCellId="0" sqref="M31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N45" activeCellId="0" sqref="N45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.26"/>
@@ -2181,11 +2184,11 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="B2" s="0" t="s">
         <v>14</v>
       </c>
@@ -2193,28 +2196,18 @@
         <v>2018</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>151</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>151</v>
+        <v>100</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>100</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <v>59.93179319</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>12.3127516778524</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>114.4817664</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="M2" s="0" t="n">
-        <v>0.22</v>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="0" t="n">
+        <v>9.4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2234,15 +2227,30 @@
         <v>151</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>59.93179319</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>58.1495726495727</v>
+        <v>12.3127516778524</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>114.4817664</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>21.1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>14</v>
@@ -2251,27 +2259,21 @@
         <v>2018</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>121</v>
+        <v>151</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>121</v>
+        <v>151</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>140.2346446</v>
+        <v>17</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>25.7815533980582</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>142.1919526</v>
+        <v>58.1495726495727</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>14</v>
@@ -2286,15 +2288,21 @@
         <v>121</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>140.2346446</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>76.4009433962264</v>
+        <v>25.7815533980582</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>142.1919526</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>14</v>
@@ -2303,13 +2311,16 @@
         <v>2018</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>76.4009433962264</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2329,13 +2340,7 @@
         <v>147</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>135.5691057</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>6.088336976</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2355,7 +2360,13 @@
         <v>147</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>135.5691057</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>6.088336976</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2375,10 +2386,7 @@
         <v>147</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>20.0629370629371</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2398,10 +2406,10 @@
         <v>147</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>9.29615547106041</v>
+        <v>20.0629370629371</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,7 +2429,10 @@
         <v>147</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>9.29615547106041</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2441,7 +2452,7 @@
         <v>147</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2461,7 +2472,7 @@
         <v>147</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,22 +2486,13 @@
         <v>2018</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>368</v>
+        <v>147</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>368</v>
+        <v>147</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <v>5.577733349</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>6.00653518496908</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>36.77803059</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2510,16 +2512,16 @@
         <v>368</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>5.577733349</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>7.78433862433862</v>
-      </c>
-      <c r="L15" s="0" t="n">
-        <v>375</v>
-      </c>
-      <c r="M15" s="0" t="n">
-        <v>12.09</v>
+        <v>6.00653518496908</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>36.77803059</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2539,10 +2541,16 @@
         <v>368</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>31.2538461538462</v>
+        <v>7.78433862433862</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>375</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>12.09</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2562,7 +2570,10 @@
         <v>368</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>31.2538461538462</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2582,7 +2593,7 @@
         <v>368</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2602,10 +2613,7 @@
         <v>368</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="0" t="n">
-        <v>7.1683748169839</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2619,22 +2627,16 @@
         <v>2018</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>586</v>
+        <v>368</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>586</v>
+        <v>368</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="0" t="n">
-        <v>8.164440297</v>
+        <v>15</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>8.00515093435553</v>
-      </c>
-      <c r="I20" s="0" t="n">
-        <v>49.69913676</v>
+        <v>7.1683748169839</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2654,10 +2656,16 @@
         <v>586</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>8.164440297</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>7.24497117232543</v>
+        <v>8.00515093435553</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>49.69913676</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2677,7 +2685,10 @@
         <v>586</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>7.24497117232543</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2697,10 +2708,7 @@
         <v>586</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="0" t="n">
-        <v>10.5844394527262</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2714,22 +2722,16 @@
         <v>2018</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>87</v>
+        <v>586</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>87</v>
+        <v>586</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="0" t="n">
-        <v>24.18012422</v>
-      </c>
       <c r="H24" s="0" t="n">
-        <v>4.72782874617737</v>
-      </c>
-      <c r="I24" s="0" t="n">
-        <v>54.81517583</v>
+        <v>10.5844394527262</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2749,16 +2751,16 @@
         <v>87</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>24.18012422</v>
       </c>
       <c r="H25" s="0" t="n">
-        <v>4.95272525027809</v>
-      </c>
-      <c r="L25" s="0" t="n">
-        <v>38.5</v>
-      </c>
-      <c r="M25" s="0" t="n">
-        <v>7.32</v>
+        <v>4.72782874617737</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>54.81517583</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2778,10 +2780,16 @@
         <v>87</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H26" s="0" t="n">
-        <v>10.8071895424837</v>
+        <v>4.95272525027809</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <v>38.5</v>
+      </c>
+      <c r="M26" s="0" t="n">
+        <v>7.32</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2795,16 +2803,16 @@
         <v>2018</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>221</v>
+        <v>87</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>221</v>
+        <v>87</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H27" s="0" t="n">
-        <v>11.6933911159263</v>
+        <v>10.8071895424837</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2824,16 +2832,10 @@
         <v>221</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H28" s="0" t="n">
-        <v>2.63057324840764</v>
-      </c>
-      <c r="L28" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="M28" s="0" t="n">
-        <v>18.46</v>
+        <v>11.6933911159263</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2853,10 +2855,16 @@
         <v>221</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H29" s="0" t="n">
-        <v>5.58258642765685</v>
+        <v>2.63057324840764</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="M29" s="0" t="n">
+        <v>18.46</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2870,22 +2878,16 @@
         <v>2018</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>85</v>
+        <v>221</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>85</v>
+        <v>221</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="0" t="n">
-        <v>26.58868425</v>
+        <v>17</v>
       </c>
       <c r="H30" s="0" t="n">
-        <v>6.12341352528888</v>
-      </c>
-      <c r="I30" s="0" t="n">
-        <v>115.1818194</v>
+        <v>5.58258642765685</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2905,16 +2907,16 @@
         <v>85</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>26.58868425</v>
       </c>
       <c r="H31" s="0" t="n">
-        <v>5.66409124356144</v>
-      </c>
-      <c r="L31" s="0" t="n">
-        <v>530</v>
-      </c>
-      <c r="M31" s="0" t="n">
-        <v>21.09</v>
+        <v>6.12341352528888</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>115.1818194</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2934,10 +2936,16 @@
         <v>85</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H32" s="0" t="n">
-        <v>13.2683760683761</v>
+        <v>5.66409124356144</v>
+      </c>
+      <c r="L32" s="0" t="n">
+        <v>530</v>
+      </c>
+      <c r="M32" s="0" t="n">
+        <v>21.09</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2957,7 +2965,10 @@
         <v>85</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <v>13.2683760683761</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2977,10 +2988,7 @@
         <v>85</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H34" s="0" t="n">
-        <v>8.43557336621455</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3000,7 +3008,10 @@
         <v>85</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <v>8.43557336621455</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3014,16 +3025,13 @@
         <v>2018</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>147</v>
+        <v>85</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>147</v>
+        <v>85</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H36" s="0" t="n">
-        <v>6.97915798249271</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3043,7 +3051,10 @@
         <v>147</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <v>6.97915798249271</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3051,33 +3062,27 @@
         <v>52</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>50</v>
+        <v>147</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>50</v>
+        <v>147</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" s="0" t="n">
-        <v>6.7035458711908</v>
-      </c>
-      <c r="I38" s="0" t="n">
-        <v>244.4055742</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>2018</v>
@@ -3089,7 +3094,13 @@
         <v>50</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>6.7035458711908</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>244.4055742</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3097,7 +3108,7 @@
         <v>55</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>2018</v>
@@ -3109,7 +3120,7 @@
         <v>50</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3117,7 +3128,7 @@
         <v>56</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>2018</v>
@@ -3129,10 +3140,7 @@
         <v>50</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H41" s="0" t="n">
-        <v>7.96274373259053</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3140,70 +3148,70 @@
         <v>57</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H42" s="0" t="n">
-        <v>6.35134728285413</v>
+        <v>7.96274373259053</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="B43" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="N43" s="0" t="n">
+        <v>45.2</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>59</v>
-      </c>
       <c r="B44" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="N44" s="0" t="n">
+        <v>42.8</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>2018</v>
@@ -3215,18 +3223,18 @@
         <v>120</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H45" s="0" t="n">
-        <v>7.10068803490519</v>
+        <v>6.35134728285413</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>2018</v>
@@ -3238,266 +3246,266 @@
         <v>120</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F47" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="G47" s="0" t="n">
-        <v>32.66219522</v>
-      </c>
-      <c r="H47" s="0" t="n">
-        <v>6.43644805571677</v>
-      </c>
-      <c r="I47" s="0" t="n">
-        <v>48.90482028</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F48" s="0" t="s">
         <v>15</v>
       </c>
       <c r="H48" s="0" t="n">
-        <v>2.96830864622804</v>
-      </c>
-      <c r="L48" s="0" t="n">
-        <v>54</v>
-      </c>
-      <c r="M48" s="0" t="n">
-        <v>9.88</v>
+        <v>7.10068803490519</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F49" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="H49" s="0" t="n">
-        <v>9.47640449438202</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G50" s="0" t="n">
-        <v>144.5962733</v>
+        <v>32.66219522</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <v>6.43644805571677</v>
       </c>
       <c r="I50" s="0" t="n">
-        <v>47.19008443</v>
+        <v>48.90482028</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>190</v>
+        <v>122</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>190</v>
+        <v>122</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="G51" s="0" t="n">
-        <v>31.86596927</v>
+        <v>17</v>
       </c>
       <c r="H51" s="0" t="n">
-        <v>5.58032128514056</v>
-      </c>
-      <c r="I51" s="0" t="n">
-        <v>24.84261045</v>
+        <v>2.96830864622804</v>
+      </c>
+      <c r="L51" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="M51" s="0" t="n">
+        <v>9.88</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>190</v>
+        <v>122</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>190</v>
+        <v>122</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H52" s="0" t="n">
-        <v>4.91321499013807</v>
-      </c>
-      <c r="L52" s="0" t="n">
-        <v>64</v>
-      </c>
-      <c r="M52" s="0" t="n">
-        <v>6.97</v>
+        <v>9.47640449438202</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C53" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>190</v>
+        <v>120</v>
       </c>
       <c r="E53" s="2" t="n">
-        <v>190</v>
+        <v>120</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H53" s="0" t="n">
-        <v>2.77491749174917</v>
+        <v>17</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <v>144.5962733</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <v>47.19008443</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C54" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>123</v>
+        <v>190</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>123</v>
+        <v>190</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G54" s="0" t="n">
-        <v>127.6422764</v>
+        <v>31.86596927</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <v>5.58032128514056</v>
+      </c>
+      <c r="I54" s="0" t="n">
+        <v>24.84261045</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>123</v>
+        <v>190</v>
       </c>
       <c r="E55" s="2" t="n">
-        <v>123</v>
+        <v>190</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <v>4.91321499013807</v>
+      </c>
+      <c r="L55" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="M55" s="0" t="n">
+        <v>6.97</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D56" s="0" t="n">
-        <v>123</v>
+        <v>190</v>
       </c>
       <c r="E56" s="2" t="n">
-        <v>123</v>
+        <v>190</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="H56" s="0" t="n">
+        <v>2.77491749174917</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C57" s="0" t="n">
         <v>2018</v>
@@ -3509,93 +3517,81 @@
         <v>123</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H57" s="0" t="n">
-        <v>8.21664180341455</v>
+        <v>15</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <v>127.6422764</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C58" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>201</v>
+        <v>123</v>
       </c>
       <c r="E58" s="2" t="n">
-        <v>201</v>
+        <v>123</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G58" s="0" t="n">
-        <v>18.53988134</v>
-      </c>
-      <c r="H58" s="0" t="n">
-        <v>6.92031090523671</v>
-      </c>
-      <c r="I58" s="0" t="n">
-        <v>206.4532045</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C59" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>201</v>
+        <v>123</v>
       </c>
       <c r="E59" s="2" t="n">
-        <v>201</v>
+        <v>123</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H59" s="0" t="n">
-        <v>13.01269035533</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C60" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>201</v>
+        <v>123</v>
       </c>
       <c r="E60" s="2" t="n">
-        <v>201</v>
+        <v>123</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H60" s="0" t="n">
-        <v>8.47593418422267</v>
+        <v>8.21664180341455</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C61" s="0" t="n">
         <v>2018</v>
@@ -3607,15 +3603,24 @@
         <v>201</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G61" s="0" t="n">
+        <v>18.53988134</v>
+      </c>
+      <c r="H61" s="0" t="n">
+        <v>6.92031090523671</v>
+      </c>
+      <c r="I61" s="0" t="n">
+        <v>206.4532045</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C62" s="0" t="n">
         <v>2018</v>
@@ -3627,15 +3632,18 @@
         <v>201</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="H62" s="0" t="n">
+        <v>13.01269035533</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C63" s="0" t="n">
         <v>2018</v>
@@ -3647,15 +3655,18 @@
         <v>201</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="H63" s="0" t="n">
+        <v>8.47593418422267</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C64" s="0" t="n">
         <v>2018</v>
@@ -3667,84 +3678,75 @@
         <v>201</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C65" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="E65" s="2" t="n">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C66" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="E66" s="2" t="n">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G66" s="0" t="n">
-        <v>7.360697997</v>
-      </c>
-      <c r="H66" s="0" t="n">
-        <v>6.82834475297512</v>
-      </c>
-      <c r="I66" s="0" t="n">
-        <v>94.40429427</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C67" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="E67" s="2" t="n">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C68" s="0" t="n">
         <v>2018</v>
@@ -3756,15 +3758,15 @@
         <v>221</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C69" s="0" t="n">
         <v>2018</v>
@@ -3776,15 +3778,24 @@
         <v>221</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G69" s="0" t="n">
+        <v>7.360697997</v>
+      </c>
+      <c r="H69" s="0" t="n">
+        <v>6.82834475297512</v>
+      </c>
+      <c r="I69" s="0" t="n">
+        <v>94.40429427</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C70" s="0" t="n">
         <v>2018</v>
@@ -3796,87 +3807,78 @@
         <v>221</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H70" s="0" t="n">
-        <v>8.58108995403808</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C71" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>586</v>
+        <v>221</v>
       </c>
       <c r="E71" s="2" t="n">
-        <v>586</v>
+        <v>221</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G71" s="0" t="n">
-        <v>5.35131205</v>
-      </c>
-      <c r="H71" s="0" t="n">
-        <v>6.19074177356386</v>
-      </c>
-      <c r="I71" s="0" t="n">
-        <v>54.4451539</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C72" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D72" s="0" t="n">
-        <v>586</v>
+        <v>221</v>
       </c>
       <c r="E72" s="2" t="n">
-        <v>586</v>
+        <v>221</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C73" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D73" s="0" t="n">
-        <v>586</v>
+        <v>221</v>
       </c>
       <c r="E73" s="2" t="n">
-        <v>586</v>
+        <v>221</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="H73" s="0" t="n">
+        <v>8.58108995403808</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C74" s="0" t="n">
         <v>2018</v>
@@ -3888,18 +3890,24 @@
         <v>586</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G74" s="0" t="n">
+        <v>5.35131205</v>
       </c>
       <c r="H74" s="0" t="n">
-        <v>9.13349633251834</v>
+        <v>6.19074177356386</v>
+      </c>
+      <c r="I74" s="0" t="n">
+        <v>54.4451539</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C75" s="0" t="n">
         <v>2018</v>
@@ -3911,275 +3919,269 @@
         <v>586</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C76" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>145</v>
+        <v>586</v>
       </c>
       <c r="E76" s="2" t="n">
-        <v>145</v>
+        <v>586</v>
       </c>
       <c r="F76" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="G76" s="0" t="n">
-        <v>16.09712027</v>
-      </c>
-      <c r="H76" s="0" t="n">
-        <v>6.04868549172347</v>
-      </c>
-      <c r="I76" s="0" t="n">
-        <v>20.25935053</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C77" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>145</v>
+        <v>586</v>
       </c>
       <c r="E77" s="2" t="n">
-        <v>145</v>
+        <v>586</v>
       </c>
       <c r="F77" s="0" t="s">
         <v>15</v>
       </c>
       <c r="H77" s="0" t="n">
-        <v>8.32882462686567</v>
-      </c>
-      <c r="L77" s="0" t="n">
-        <v>181</v>
-      </c>
-      <c r="M77" s="0" t="n">
-        <v>7.36</v>
+        <v>9.13349633251834</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C78" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>145</v>
+        <v>586</v>
       </c>
       <c r="E78" s="2" t="n">
-        <v>145</v>
+        <v>586</v>
       </c>
       <c r="F78" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="H78" s="0" t="n">
-        <v>12.3678756476684</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C79" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>288</v>
+        <v>145</v>
       </c>
       <c r="E79" s="2" t="n">
-        <v>288</v>
+        <v>145</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G79" s="0" t="n">
-        <v>9.216589862</v>
+        <v>16.09712027</v>
       </c>
       <c r="H79" s="0" t="n">
-        <v>7.42969396195203</v>
+        <v>6.04868549172347</v>
       </c>
       <c r="I79" s="0" t="n">
-        <v>113.4440422</v>
+        <v>20.25935053</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C80" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D80" s="0" t="n">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="E80" s="2" t="n">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="G80" s="0" t="n">
-        <v>13.12777285</v>
+        <v>17</v>
       </c>
       <c r="H80" s="0" t="n">
-        <v>9.40529531568228</v>
-      </c>
-      <c r="I80" s="0" t="n">
-        <v>29.19970064</v>
+        <v>8.32882462686567</v>
+      </c>
+      <c r="L80" s="0" t="n">
+        <v>181</v>
+      </c>
+      <c r="M80" s="0" t="n">
+        <v>7.36</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C81" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="E81" s="2" t="n">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H81" s="0" t="n">
-        <v>8.89652777777778</v>
-      </c>
-      <c r="L81" s="0" t="n">
-        <v>160</v>
-      </c>
-      <c r="M81" s="0" t="n">
-        <v>12.96</v>
+        <v>12.3678756476684</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C82" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D82" s="0" t="n">
-        <v>93</v>
+        <v>288</v>
       </c>
       <c r="E82" s="2" t="n">
-        <v>93</v>
+        <v>288</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="G82" s="0" t="n">
+        <v>9.216589862</v>
       </c>
       <c r="H82" s="0" t="n">
-        <v>10.8880952380952</v>
+        <v>7.42969396195203</v>
+      </c>
+      <c r="I82" s="0" t="n">
+        <v>113.4440422</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C83" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D83" s="0" t="n">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="E83" s="2" t="n">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G83" s="0" t="n">
-        <v>54.63414634</v>
+        <v>13.12777285</v>
       </c>
       <c r="H83" s="0" t="n">
-        <v>12.2922794117647</v>
+        <v>9.40529531568228</v>
       </c>
       <c r="I83" s="0" t="n">
-        <v>44.60837344</v>
+        <v>29.19970064</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C84" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D84" s="0" t="n">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="E84" s="2" t="n">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="H84" s="0" t="n">
+        <v>8.89652777777778</v>
+      </c>
+      <c r="L84" s="0" t="n">
+        <v>160</v>
+      </c>
+      <c r="M84" s="0" t="n">
+        <v>12.96</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C85" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D85" s="0" t="n">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="E85" s="2" t="n">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="H85" s="0" t="n">
+        <v>10.8880952380952</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C86" s="0" t="n">
         <v>2018</v>
@@ -4191,15 +4193,24 @@
         <v>143</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G86" s="0" t="n">
+        <v>54.63414634</v>
+      </c>
+      <c r="H86" s="0" t="n">
+        <v>12.2922794117647</v>
+      </c>
+      <c r="I86" s="0" t="n">
+        <v>44.60837344</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C87" s="0" t="n">
         <v>2018</v>
@@ -4211,18 +4222,15 @@
         <v>143</v>
       </c>
       <c r="F87" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H87" s="0" t="n">
-        <v>8.09428794992175</v>
+        <v>15</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C88" s="0" t="n">
         <v>2018</v>
@@ -4234,81 +4242,78 @@
         <v>143</v>
       </c>
       <c r="F88" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C89" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D89" s="0" t="n">
-        <v>843</v>
+        <v>143</v>
       </c>
       <c r="E89" s="2" t="n">
-        <v>843</v>
+        <v>143</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H89" s="0" t="n">
-        <v>4.51894411621226</v>
-      </c>
-      <c r="I89" s="0" t="n">
-        <v>28.51596639</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C90" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D90" s="0" t="n">
-        <v>843</v>
+        <v>143</v>
       </c>
       <c r="E90" s="2" t="n">
-        <v>843</v>
+        <v>143</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="H90" s="0" t="n">
+        <v>8.09428794992175</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C91" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D91" s="0" t="n">
-        <v>843</v>
+        <v>143</v>
       </c>
       <c r="E91" s="2" t="n">
-        <v>843</v>
+        <v>143</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C92" s="0" t="n">
         <v>2018</v>
@@ -4320,15 +4325,21 @@
         <v>843</v>
       </c>
       <c r="F92" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="H92" s="0" t="n">
+        <v>4.51894411621226</v>
+      </c>
+      <c r="I92" s="0" t="n">
+        <v>28.51596639</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C93" s="0" t="n">
         <v>2018</v>
@@ -4340,9 +4351,69 @@
         <v>843</v>
       </c>
       <c r="F93" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H93" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C94" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <v>843</v>
+      </c>
+      <c r="E94" s="2" t="n">
+        <v>843</v>
+      </c>
+      <c r="F94" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C95" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <v>843</v>
+      </c>
+      <c r="E95" s="2" t="n">
+        <v>843</v>
+      </c>
+      <c r="F95" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C96" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D96" s="0" t="n">
+        <v>843</v>
+      </c>
+      <c r="E96" s="2" t="n">
+        <v>843</v>
+      </c>
+      <c r="F96" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H96" s="0" t="n">
         <v>8.58502772643253</v>
       </c>
     </row>
@@ -4368,25 +4439,25 @@
       <selection pane="topLeft" activeCell="T38" activeCellId="0" sqref="T38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>50</v>
@@ -4401,7 +4472,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>93</v>
@@ -4416,7 +4487,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>120</v>
@@ -4431,7 +4502,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>122</v>
@@ -4446,7 +4517,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>143</v>
@@ -4461,7 +4532,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>145</v>
@@ -4476,7 +4547,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>190</v>
@@ -4491,7 +4562,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>201</v>
@@ -4506,7 +4577,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>221</v>
@@ -4521,7 +4592,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>288</v>
@@ -4536,7 +4607,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>586</v>
@@ -4551,7 +4622,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>843</v>
@@ -4569,13 +4640,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
no more titles on plots
</commit_message>
<xml_diff>
--- a/data/flux/2018-fluxes.xlsx
+++ b/data/flux/2018-fluxes.xlsx
@@ -544,7 +544,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart140.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -745,11 +745,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="27447601"/>
-        <c:axId val="65623402"/>
+        <c:axId val="12221273"/>
+        <c:axId val="35166984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="27447601"/>
+        <c:axId val="12221273"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -805,12 +805,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65623402"/>
+        <c:crossAx val="35166984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65623402"/>
+        <c:axId val="35166984"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -875,7 +875,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27447601"/>
+        <c:crossAx val="12221273"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -923,7 +923,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart141.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1094,11 +1094,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="41869196"/>
-        <c:axId val="29199994"/>
+        <c:axId val="22980108"/>
+        <c:axId val="36867245"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="41869196"/>
+        <c:axId val="22980108"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1154,12 +1154,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29199994"/>
+        <c:crossAx val="36867245"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="29199994"/>
+        <c:axId val="36867245"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1224,7 +1224,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41869196"/>
+        <c:crossAx val="22980108"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1272,7 +1272,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart142.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart49.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1473,11 +1473,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="1200342"/>
-        <c:axId val="32779726"/>
+        <c:axId val="85053520"/>
+        <c:axId val="2510107"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1200342"/>
+        <c:axId val="85053520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1533,12 +1533,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32779726"/>
+        <c:crossAx val="2510107"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="32779726"/>
+        <c:axId val="2510107"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1603,7 +1603,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1200342"/>
+        <c:crossAx val="85053520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1651,7 +1651,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart143.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart50.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1822,11 +1822,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="43754104"/>
-        <c:axId val="52110172"/>
+        <c:axId val="30073782"/>
+        <c:axId val="50921259"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43754104"/>
+        <c:axId val="30073782"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1882,12 +1882,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52110172"/>
+        <c:crossAx val="50921259"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52110172"/>
+        <c:axId val="50921259"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1952,7 +1952,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43754104"/>
+        <c:crossAx val="30073782"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2011,9 +2011,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>716760</xdr:colOff>
+      <xdr:colOff>716400</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>82800</xdr:rowOff>
+      <xdr:rowOff>82440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2021,8 +2021,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5114880" y="86040"/>
-        <a:ext cx="5484960" cy="4548240"/>
+        <a:off x="5122440" y="86040"/>
+        <a:ext cx="5492160" cy="4547880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2041,9 +2041,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>223200</xdr:colOff>
+      <xdr:colOff>222840</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>54360</xdr:rowOff>
+      <xdr:rowOff>54000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2051,8 +2051,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5108040" y="4924800"/>
-        <a:ext cx="4998240" cy="4720320"/>
+        <a:off x="5115600" y="4924800"/>
+        <a:ext cx="5005440" cy="4719960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2071,9 +2071,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>603000</xdr:colOff>
+      <xdr:colOff>602640</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>159120</xdr:rowOff>
+      <xdr:rowOff>158760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2081,8 +2081,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10766160" y="0"/>
-        <a:ext cx="5484960" cy="4548240"/>
+        <a:off x="10782720" y="0"/>
+        <a:ext cx="5492160" cy="4547880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2101,9 +2101,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>96480</xdr:colOff>
+      <xdr:colOff>96120</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>102240</xdr:rowOff>
+      <xdr:rowOff>101880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2111,8 +2111,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10746360" y="4972680"/>
-        <a:ext cx="4998240" cy="4720320"/>
+        <a:off x="10762920" y="4972680"/>
+        <a:ext cx="5005440" cy="4719960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2133,10 +2133,10 @@
   <dimension ref="A1:O96"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M80" activeCellId="0" sqref="M80"/>
+      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.26"/>
@@ -4482,7 +4482,7 @@
       <selection pane="topLeft" activeCell="T38" activeCellId="0" sqref="T38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
tried to unipept 100 m sus fungi
</commit_message>
<xml_diff>
--- a/data/flux/2018-fluxes.xlsx
+++ b/data/flux/2018-fluxes.xlsx
@@ -1251,7 +1251,1084 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>2018 P2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'martin power law'!$C$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fz C flux organic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'martin power law'!$C$17:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>115.1818194</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54.81517583</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>142.1919526</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.088336976</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>114.4817664</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36.77803059</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>49.69913676</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'martin power law'!$B$17:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>368</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>586</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="44750915"/>
+        <c:axId val="14021547"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="44750915"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Org C flux (umol/m2/day0</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="14021547"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="14021547"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="44750915"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>2018 P1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'martin power law'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fz C flux organic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'martin power law'!$D$2:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>15.6987637849462</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.19970064</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37.677033083871</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38.3049836352688</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44.8984644249462</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45.5264149763441</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59.6553023827957</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>63.1090304154839</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>69.3885359294624</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90.4248794012903</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>183.98951155957</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>264.681157414194</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'martin power law'!$C$2:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>244.4055742</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.19970064</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47.19008443</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48.90482028</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44.60837344</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.25935053</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.84261045</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>206.4532045</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>94.40429427</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>113.4440422</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>54.4451539</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28.51596639</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="1699133"/>
+        <c:axId val="6883477"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1699133"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Org C flux (umol C/m2/day)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="6883477"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="6883477"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1699133"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>2018 P2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'martin power law'!$C$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fz C flux organic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'martin power law'!$D$17:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>53.5550568454023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54.81517583</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>76.2371985681609</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>92.6187453679311</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95.1389833371264</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>231.861893165977</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>369.214862487126</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'martin power law'!$C$17:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>115.1818194</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54.81517583</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>142.1919526</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.088336976</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>114.4817664</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36.77803059</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>49.69913676</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="1720729"/>
+        <c:axId val="32534370"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1720729"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Org C flux (umol/m2/day0</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="32534370"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="32534370"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1720729"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1452,11 +2529,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="64439864"/>
-        <c:axId val="29484826"/>
+        <c:axId val="3519189"/>
+        <c:axId val="40360850"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64439864"/>
+        <c:axId val="3519189"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1512,12 +2589,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29484826"/>
+        <c:crossAx val="40360850"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="29484826"/>
+        <c:axId val="40360850"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1582,1085 +2659,8 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64439864"/>
+        <c:crossAx val="3519189"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="0">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>2018 P2</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'martin power law'!$C$16</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Fz C flux organic</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="0">
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'martin power law'!$C$17:$C$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>115.1818194</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>54.81517583</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>142.1919526</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.088336976</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>114.4817664</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>36.77803059</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>49.69913676</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'martin power law'!$B$17:$B$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>121</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>147</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>151</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>368</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>586</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:axId val="13887672"/>
-        <c:axId val="95168473"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="13887672"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Org C flux (umol/m2/day0</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="95168473"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="95168473"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Depth (m)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="13887672"/>
-        <c:crossesAt val="0"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="0">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>2018 P1</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'martin power law'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Fz C flux organic</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="0">
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'martin power law'!$D$2:$D$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>15.6987637849462</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>29.19970064</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>37.677033083871</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>38.3049836352688</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>44.8984644249462</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45.5264149763441</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>59.6553023827957</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>63.1090304154839</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>69.3885359294624</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>90.4248794012903</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>183.98951155957</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>264.681157414194</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'martin power law'!$C$2:$C$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>244.4055742</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>29.19970064</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>47.19008443</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>48.90482028</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>44.60837344</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>20.25935053</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24.84261045</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>206.4532045</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>94.40429427</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>113.4440422</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>54.4451539</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>28.51596639</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:axId val="40488500"/>
-        <c:axId val="42386068"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="40488500"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Org C flux (umol C/m2/day)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="42386068"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="42386068"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Depth (m)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="40488500"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="0">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>2018 P2</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'martin power law'!$C$16</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Fz C flux organic</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="0">
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'martin power law'!$D$17:$D$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>53.5550568454023</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>54.81517583</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>76.2371985681609</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>92.6187453679311</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>95.1389833371264</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>231.861893165977</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>369.214862487126</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'martin power law'!$C$17:$C$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>115.1818194</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>54.81517583</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>142.1919526</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.088336976</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>114.4817664</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>36.77803059</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>49.69913676</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:axId val="1931826"/>
-        <c:axId val="41028811"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1931826"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Org C flux (umol/m2/day0</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="41028811"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="41028811"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Depth (m)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1931826"/>
-        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2839,8 +2839,8 @@
   </sheetPr>
   <dimension ref="A1:Q96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P92" activeCellId="0" sqref="P92"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P93" activeCellId="0" sqref="P93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3462,6 +3462,9 @@
       <c r="H24" s="0" t="n">
         <v>10.5844394527262</v>
       </c>
+      <c r="P24" s="0" t="n">
+        <v>17.77</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
@@ -3889,6 +3892,9 @@
       <c r="F41" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="P41" s="0" t="n">
+        <v>10.35</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
@@ -5138,6 +5144,9 @@
       </c>
       <c r="F93" s="0" t="s">
         <v>18</v>
+      </c>
+      <c r="P93" s="0" t="n">
+        <v>15.82</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5559,8 +5568,8 @@
   </sheetPr>
   <dimension ref="A1:M215"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K97" activeCellId="0" sqref="K97"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A115" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K137" activeCellId="0" sqref="K137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
221top 2018 p2 not showing in plot
</commit_message>
<xml_diff>
--- a/data/flux/2018-fluxes.xlsx
+++ b/data/flux/2018-fluxes.xlsx
@@ -1285,7 +1285,386 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart100.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>2018 P1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'martin power law'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fz C flux organic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'martin power law'!$C$2:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>244.4055742</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.19970064</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47.19008443</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48.90482028</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44.60837344</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.25935053</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.84261045</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>206.4532045</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>94.40429427</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>113.4440422</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>54.4451539</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28.51596639</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'martin power law'!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>586</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>843</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="84174626"/>
+        <c:axId val="98419843"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="84174626"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Org C flux (umol C/m2/day)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="98419843"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="98419843"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="84174626"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1456,11 +1835,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="43284399"/>
-        <c:axId val="35112559"/>
+        <c:axId val="44255887"/>
+        <c:axId val="13532329"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43284399"/>
+        <c:axId val="44255887"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1516,12 +1895,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35112559"/>
+        <c:crossAx val="13532329"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="35112559"/>
+        <c:axId val="13532329"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1586,7 +1965,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43284399"/>
+        <c:crossAx val="44255887"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1634,7 +2013,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart101.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1835,11 +2214,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="13047167"/>
-        <c:axId val="26506460"/>
+        <c:axId val="34273245"/>
+        <c:axId val="77235741"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="13047167"/>
+        <c:axId val="34273245"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1895,12 +2274,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26506460"/>
+        <c:crossAx val="77235741"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="26506460"/>
+        <c:axId val="77235741"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1965,7 +2344,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13047167"/>
+        <c:crossAx val="34273245"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2013,7 +2392,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart102.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2184,11 +2563,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="76102035"/>
-        <c:axId val="65838917"/>
+        <c:axId val="41561160"/>
+        <c:axId val="95620272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76102035"/>
+        <c:axId val="41561160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2244,12 +2623,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65838917"/>
+        <c:crossAx val="95620272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65838917"/>
+        <c:axId val="95620272"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2314,387 +2693,8 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76102035"/>
+        <c:crossAx val="41561160"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="0">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart99.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>2018 P1</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'martin power law'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Fz C flux organic</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="0">
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'martin power law'!$C$2:$C$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>244.4055742</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>29.19970064</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>47.19008443</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>48.90482028</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>44.60837344</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>20.25935053</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24.84261045</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>206.4532045</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>94.40429427</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>113.4440422</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>54.4451539</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>28.51596639</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'martin power law'!$B$2:$B$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>122</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>143</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>201</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>221</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>288</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>586</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>843</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:axId val="23969576"/>
-        <c:axId val="56645242"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="23969576"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Org C flux (umol C/m2/day)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="56645242"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="56645242"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Depth (m)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="23969576"/>
-        <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2752,9 +2752,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>714240</xdr:colOff>
+      <xdr:colOff>713880</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:rowOff>79920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2762,8 +2762,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5164560" y="86040"/>
-        <a:ext cx="5531760" cy="4546080"/>
+        <a:off x="5172120" y="86040"/>
+        <a:ext cx="5539320" cy="4545720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2782,9 +2782,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>220680</xdr:colOff>
+      <xdr:colOff>220320</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>51840</xdr:rowOff>
+      <xdr:rowOff>51480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2792,8 +2792,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5157720" y="4925160"/>
-        <a:ext cx="5045040" cy="4717800"/>
+        <a:off x="5165280" y="4925160"/>
+        <a:ext cx="5052600" cy="4717440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2812,9 +2812,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>600480</xdr:colOff>
+      <xdr:colOff>600120</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>156240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2822,8 +2822,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10873800" y="0"/>
-        <a:ext cx="5531760" cy="4545720"/>
+        <a:off x="10890360" y="0"/>
+        <a:ext cx="5538960" cy="4545360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2842,9 +2842,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>93960</xdr:colOff>
+      <xdr:colOff>93600</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>99720</xdr:rowOff>
+      <xdr:rowOff>99360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2852,8 +2852,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10854000" y="4973040"/>
-        <a:ext cx="5045040" cy="4717800"/>
+        <a:off x="10870560" y="4973040"/>
+        <a:ext cx="5052240" cy="4717440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2873,11 +2873,11 @@
   </sheetPr>
   <dimension ref="A1:T96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S23" activeCellId="0" sqref="S23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.26"/>
@@ -6149,7 +6149,7 @@
       <selection pane="topLeft" activeCell="T38" activeCellId="0" sqref="T38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -6487,7 +6487,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="14.16"/>
@@ -12835,7 +12835,7 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="14.16"/>

</xml_diff>

<commit_message>
adding in 2012 sinking fluxes excel
</commit_message>
<xml_diff>
--- a/data/flux/2018-fluxes.xlsx
+++ b/data/flux/2018-fluxes.xlsx
@@ -1306,7 +1306,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart105.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart109.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1507,11 +1507,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="74669475"/>
-        <c:axId val="6802735"/>
+        <c:axId val="99718784"/>
+        <c:axId val="40170162"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74669475"/>
+        <c:axId val="99718784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1567,12 +1567,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6802735"/>
+        <c:crossAx val="40170162"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="6802735"/>
+        <c:axId val="40170162"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1637,7 +1637,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74669475"/>
+        <c:crossAx val="99718784"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1685,7 +1685,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart106.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart110.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1856,11 +1856,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="69378014"/>
-        <c:axId val="64632802"/>
+        <c:axId val="19680016"/>
+        <c:axId val="21145269"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69378014"/>
+        <c:axId val="19680016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1916,12 +1916,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64632802"/>
+        <c:crossAx val="21145269"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64632802"/>
+        <c:axId val="21145269"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1986,7 +1986,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69378014"/>
+        <c:crossAx val="19680016"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2034,7 +2034,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart107.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart111.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2235,11 +2235,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="5955580"/>
-        <c:axId val="31380799"/>
+        <c:axId val="14300129"/>
+        <c:axId val="79458895"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="5955580"/>
+        <c:axId val="14300129"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2295,12 +2295,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31380799"/>
+        <c:crossAx val="79458895"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="31380799"/>
+        <c:axId val="79458895"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2365,7 +2365,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5955580"/>
+        <c:crossAx val="14300129"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2413,7 +2413,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart108.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart112.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2584,11 +2584,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="72166527"/>
-        <c:axId val="1766882"/>
+        <c:axId val="60110363"/>
+        <c:axId val="47368539"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72166527"/>
+        <c:axId val="60110363"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2644,12 +2644,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1766882"/>
+        <c:crossAx val="47368539"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1766882"/>
+        <c:axId val="47368539"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2714,7 +2714,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72166527"/>
+        <c:crossAx val="60110363"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>